<commit_message>
Laborator 07.10.2024 - citire si afisare graf
</commit_message>
<xml_diff>
--- a/MetodeAvansateDeProgramare/Prezenta_AnII_2024.xlsx
+++ b/MetodeAvansateDeProgramare/Prezenta_AnII_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_Promotia_2023_2026\MetodeAvansateDeProgramare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C9D84E9-4399-4427-8739-1B5C24F271C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD303B7F-B049-416E-8366-FDECA6C733E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Proiect</t>
   </si>
@@ -103,6 +103,18 @@
   </si>
   <si>
     <t>Cătălin Lazăr</t>
+  </si>
+  <si>
+    <t>Vanesa Clepce</t>
+  </si>
+  <si>
+    <t>Bianca Abrudan</t>
+  </si>
+  <si>
+    <t>Andrei Mâța</t>
+  </si>
+  <si>
+    <t>Roland Roman</t>
   </si>
 </sst>
 </file>
@@ -358,7 +370,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -437,7 +449,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -449,19 +460,7 @@
     <cellStyle name="Default" xfId="1" xr:uid="{EB53C024-DCAD-4D39-B7BA-74E17CBDBE71}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF000000"/>
-        <family val="2"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF7C80"/>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -751,7 +750,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I14" sqref="I14"/>
+      <selection pane="bottomRight" activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -843,8 +842,8 @@
         <f>C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
         <v>1</v>
       </c>
-      <c r="R3" s="37"/>
-      <c r="S3" s="38"/>
+      <c r="R3" s="36"/>
+      <c r="S3" s="37"/>
     </row>
     <row r="4" spans="2:19">
       <c r="B4" s="3" t="s">
@@ -864,7 +863,7 @@
     </row>
     <row r="5" spans="2:19">
       <c r="B5" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C5" s="8" t="b">
         <v>1</v>
@@ -880,7 +879,7 @@
     </row>
     <row r="6" spans="2:19">
       <c r="B6" s="3" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C6" s="8" t="b">
         <v>1</v>
@@ -895,51 +894,29 @@
       <c r="S6" s="11"/>
     </row>
     <row r="7" spans="2:19">
-      <c r="B7" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
+      <c r="B7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="8" t="b">
+        <v>1</v>
+      </c>
       <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="21"/>
-      <c r="O7" s="21"/>
-      <c r="P7" s="24"/>
+      <c r="P7" s="9"/>
       <c r="Q7" s="7">
         <f>C7+D7+E7+F7+G7+H7+I7+J7+K7+L7+M7+N7+O7+P7</f>
         <v>1</v>
       </c>
-      <c r="R7" s="26"/>
-      <c r="S7" s="34"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="11"/>
     </row>
     <row r="8" spans="2:19">
       <c r="B8" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="36"/>
       <c r="J8" s="21"/>
-      <c r="K8" s="36"/>
-      <c r="L8" s="36"/>
-      <c r="M8" s="36"/>
-      <c r="N8" s="36"/>
-      <c r="O8" s="36"/>
       <c r="P8" s="9"/>
       <c r="Q8" s="7">
         <f>C8+D8+E8+F8+G8+H8+I8+J8+K8+L8+M8+N8+O8+P8</f>
@@ -949,24 +926,35 @@
       <c r="S8" s="11"/>
     </row>
     <row r="9" spans="2:19">
-      <c r="B9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="8" t="b">
-        <v>1</v>
-      </c>
+      <c r="B9" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
       <c r="J9" s="21"/>
-      <c r="P9" s="9"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="24"/>
       <c r="Q9" s="7">
         <f>C9+D9+E9+F9+G9+H9+I9+J9+K9+L9+M9+N9+O9+P9</f>
         <v>1</v>
       </c>
-      <c r="R9" s="12"/>
-      <c r="S9" s="13"/>
+      <c r="R9" s="26"/>
+      <c r="S9" s="34"/>
     </row>
     <row r="10" spans="2:19">
       <c r="B10" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C10" s="8" t="b">
         <v>1</v>
@@ -981,49 +969,65 @@
       <c r="S10" s="11"/>
     </row>
     <row r="11" spans="2:19">
-      <c r="B11" s="3"/>
-      <c r="C11" s="8"/>
+      <c r="B11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="8" t="b">
+        <v>1</v>
+      </c>
       <c r="J11" s="21"/>
       <c r="P11" s="9"/>
       <c r="Q11" s="7">
-        <f t="shared" ref="Q4:Q57" si="0">C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11+P11</f>
-        <v>0</v>
-      </c>
-      <c r="R11" s="10"/>
-      <c r="S11" s="11"/>
+        <f>C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11+P11</f>
+        <v>1</v>
+      </c>
+      <c r="R11" s="12"/>
+      <c r="S11" s="13"/>
     </row>
     <row r="12" spans="2:19">
-      <c r="B12" s="3"/>
-      <c r="C12" s="8"/>
+      <c r="B12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="8" t="b">
+        <v>1</v>
+      </c>
       <c r="J12" s="21"/>
       <c r="P12" s="9"/>
       <c r="Q12" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12+P12</f>
+        <v>1</v>
       </c>
       <c r="R12" s="10"/>
       <c r="S12" s="11"/>
     </row>
     <row r="13" spans="2:19">
-      <c r="B13" s="3"/>
-      <c r="C13" s="8"/>
+      <c r="B13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="8" t="b">
+        <v>1</v>
+      </c>
       <c r="J13" s="21"/>
       <c r="P13" s="9"/>
       <c r="Q13" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13+P13</f>
+        <v>1</v>
       </c>
       <c r="R13" s="10"/>
       <c r="S13" s="11"/>
     </row>
     <row r="14" spans="2:19">
-      <c r="B14" s="3"/>
-      <c r="C14" s="8"/>
+      <c r="B14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="8" t="b">
+        <v>1</v>
+      </c>
       <c r="J14" s="21"/>
       <c r="P14" s="9"/>
       <c r="Q14" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14+P14</f>
+        <v>1</v>
       </c>
       <c r="R14" s="10"/>
       <c r="S14" s="11"/>
@@ -1034,7 +1038,7 @@
       <c r="J15" s="21"/>
       <c r="P15" s="9"/>
       <c r="Q15" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="Q11:Q57" si="0">C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15+P15</f>
         <v>0</v>
       </c>
       <c r="R15" s="12"/>
@@ -1600,11 +1604,11 @@
       <c r="S57" s="18"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S10">
-    <sortCondition ref="B3:B10"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S14">
+    <sortCondition ref="B3:B14"/>
   </sortState>
   <conditionalFormatting sqref="Q3:Q57">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Laborator 08.10.2024 - inceputul unei aplicatii web, cu doar HTML si CSS
</commit_message>
<xml_diff>
--- a/MetodeAvansateDeProgramare/Prezenta_AnII_2024.xlsx
+++ b/MetodeAvansateDeProgramare/Prezenta_AnII_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_Promotia_2023_2026\MetodeAvansateDeProgramare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD303B7F-B049-416E-8366-FDECA6C733E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163F651E-6AA1-4503-8B0F-DBC92CDCD5E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Proiect</t>
   </si>
@@ -115,6 +115,42 @@
   </si>
   <si>
     <t>Roland Roman</t>
+  </si>
+  <si>
+    <t>Nicolae Goia</t>
+  </si>
+  <si>
+    <t>Erik Lazin</t>
+  </si>
+  <si>
+    <t>Raul Hollo</t>
+  </si>
+  <si>
+    <t>Daria Petre</t>
+  </si>
+  <si>
+    <t>Gabriel Talmazan</t>
+  </si>
+  <si>
+    <t>George Vezentan</t>
+  </si>
+  <si>
+    <t>Renata Tirban</t>
+  </si>
+  <si>
+    <t>AnaMaria  Bohar</t>
+  </si>
+  <si>
+    <t>Cristina Nemcea</t>
+  </si>
+  <si>
+    <t>Diana Lazea</t>
+  </si>
+  <si>
+    <t>Boglarka Szigeti</t>
+  </si>
+  <si>
+    <t>Daria Puscas</t>
   </si>
 </sst>
 </file>
@@ -747,7 +783,7 @@
   <dimension ref="B2:S57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="J18" sqref="J18"/>
@@ -825,7 +861,9 @@
       <c r="C3" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="D3" s="5"/>
+      <c r="D3" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
@@ -839,8 +877,8 @@
       <c r="O3" s="5"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="7">
-        <f>C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
-        <v>1</v>
+        <f t="shared" ref="Q3:Q14" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
+        <v>2</v>
       </c>
       <c r="R3" s="36"/>
       <c r="S3" s="37"/>
@@ -855,7 +893,7 @@
       <c r="J4" s="21"/>
       <c r="P4" s="9"/>
       <c r="Q4" s="7">
-        <f>C4+D4+E4+F4+G4+H4+I4+J4+K4+L4+M4+N4+O4+P4</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R4" s="10"/>
@@ -865,13 +903,14 @@
       <c r="B5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="8" t="b">
+      <c r="C5" s="8"/>
+      <c r="D5" t="b">
         <v>1</v>
       </c>
       <c r="J5" s="21"/>
       <c r="P5" s="9"/>
       <c r="Q5" s="7">
-        <f>C5+D5+E5+F5+G5+H5+I5+J5+K5+L5+M5+N5+O5+P5</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R5" s="10"/>
@@ -881,13 +920,14 @@
       <c r="B6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="8" t="b">
+      <c r="C6" s="8"/>
+      <c r="D6" t="b">
         <v>1</v>
       </c>
       <c r="J6" s="21"/>
       <c r="P6" s="9"/>
       <c r="Q6" s="7">
-        <f>C6+D6+E6+F6+G6+H6+I6+J6+K6+L6+M6+N6+O6+P6</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R6" s="10"/>
@@ -903,7 +943,7 @@
       <c r="J7" s="21"/>
       <c r="P7" s="9"/>
       <c r="Q7" s="7">
-        <f>C7+D7+E7+F7+G7+H7+I7+J7+K7+L7+M7+N7+O7+P7</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R7" s="10"/>
@@ -916,47 +956,41 @@
       <c r="C8" s="8" t="b">
         <v>1</v>
       </c>
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
       <c r="J8" s="21"/>
       <c r="P8" s="9"/>
       <c r="Q8" s="7">
-        <f>C8+D8+E8+F8+G8+H8+I8+J8+K8+L8+M8+N8+O8+P8</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="R8" s="10"/>
       <c r="S8" s="11"/>
     </row>
     <row r="9" spans="2:19">
-      <c r="B9" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
+      <c r="B9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
       <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="21"/>
-      <c r="O9" s="21"/>
-      <c r="P9" s="24"/>
+      <c r="P9" s="9"/>
       <c r="Q9" s="7">
         <f>C9+D9+E9+F9+G9+H9+I9+J9+K9+L9+M9+N9+O9+P9</f>
         <v>1</v>
       </c>
-      <c r="R9" s="26"/>
-      <c r="S9" s="34"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="11"/>
     </row>
     <row r="10" spans="2:19">
       <c r="B10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="8" t="b">
+        <v>40</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" t="b">
         <v>1</v>
       </c>
       <c r="J10" s="21"/>
@@ -970,9 +1004,10 @@
     </row>
     <row r="11" spans="2:19">
       <c r="B11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="8" t="b">
+        <v>38</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" t="b">
         <v>1</v>
       </c>
       <c r="J11" s="21"/>
@@ -981,14 +1016,15 @@
         <f>C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11+P11</f>
         <v>1</v>
       </c>
-      <c r="R11" s="12"/>
-      <c r="S11" s="13"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="11"/>
     </row>
     <row r="12" spans="2:19">
       <c r="B12" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="8" t="b">
+        <v>33</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" t="b">
         <v>1</v>
       </c>
       <c r="J12" s="21"/>
@@ -1001,191 +1037,264 @@
       <c r="S12" s="11"/>
     </row>
     <row r="13" spans="2:19">
-      <c r="B13" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="8" t="b">
-        <v>1</v>
-      </c>
+      <c r="B13" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="23"/>
+      <c r="D13" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
       <c r="J13" s="21"/>
-      <c r="P13" s="9"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="21"/>
+      <c r="P13" s="24"/>
       <c r="Q13" s="7">
         <f>C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13+P13</f>
         <v>1</v>
       </c>
-      <c r="R13" s="10"/>
-      <c r="S13" s="11"/>
+      <c r="R13" s="26"/>
+      <c r="S13" s="34"/>
     </row>
     <row r="14" spans="2:19">
-      <c r="B14" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="8" t="b">
-        <v>1</v>
-      </c>
+      <c r="B14" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
       <c r="J14" s="21"/>
-      <c r="P14" s="9"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="24"/>
       <c r="Q14" s="7">
         <f>C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14+P14</f>
-        <v>1</v>
-      </c>
-      <c r="R14" s="10"/>
-      <c r="S14" s="11"/>
+        <v>2</v>
+      </c>
+      <c r="R14" s="26"/>
+      <c r="S14" s="34"/>
     </row>
     <row r="15" spans="2:19">
-      <c r="B15" s="3"/>
+      <c r="B15" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="C15" s="8"/>
+      <c r="D15" t="b">
+        <v>1</v>
+      </c>
       <c r="J15" s="21"/>
       <c r="P15" s="9"/>
       <c r="Q15" s="7">
-        <f t="shared" ref="Q11:Q57" si="0">C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15+P15</f>
-        <v>0</v>
-      </c>
-      <c r="R15" s="12"/>
-      <c r="S15" s="13"/>
+        <f>C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15+P15</f>
+        <v>1</v>
+      </c>
+      <c r="R15" s="10"/>
+      <c r="S15" s="11"/>
     </row>
     <row r="16" spans="2:19">
-      <c r="B16" s="3"/>
+      <c r="B16" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="C16" s="8"/>
+      <c r="D16" t="b">
+        <v>1</v>
+      </c>
       <c r="J16" s="21"/>
       <c r="P16" s="9"/>
       <c r="Q16" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>C16+D16+E16+F16+G16+H16+I16+J16+K16+L16+M16+N16+O16+P16</f>
+        <v>1</v>
       </c>
       <c r="R16" s="12"/>
       <c r="S16" s="13"/>
     </row>
     <row r="17" spans="2:19">
-      <c r="B17" s="3"/>
+      <c r="B17" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="C17" s="8"/>
+      <c r="D17" t="b">
+        <v>1</v>
+      </c>
       <c r="J17" s="21"/>
       <c r="P17" s="9"/>
       <c r="Q17" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17+P17</f>
+        <v>1</v>
       </c>
       <c r="R17" s="10"/>
       <c r="S17" s="11"/>
     </row>
     <row r="18" spans="2:19">
-      <c r="B18" s="3"/>
+      <c r="B18" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="C18" s="8"/>
+      <c r="D18" t="b">
+        <v>1</v>
+      </c>
       <c r="J18" s="21"/>
       <c r="P18" s="9"/>
       <c r="Q18" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>C18+D18+E18+F18+G18+H18+I18+J18+K18+L18+M18+N18+O18+P18</f>
+        <v>1</v>
       </c>
       <c r="R18" s="10"/>
       <c r="S18" s="11"/>
     </row>
     <row r="19" spans="2:19">
-      <c r="B19" s="3"/>
+      <c r="B19" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="C19" s="8"/>
+      <c r="D19" t="b">
+        <v>1</v>
+      </c>
       <c r="J19" s="21"/>
       <c r="P19" s="9"/>
       <c r="Q19" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R19" s="10"/>
-      <c r="S19" s="11"/>
+        <f>C19+D19+E19+F19+G19+H19+I19+J19+K19+L19+M19+N19+O19+P19</f>
+        <v>1</v>
+      </c>
+      <c r="R19" s="12"/>
+      <c r="S19" s="13"/>
     </row>
     <row r="20" spans="2:19">
-      <c r="B20" s="3"/>
-      <c r="C20" s="8"/>
+      <c r="B20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="8" t="b">
+        <v>1</v>
+      </c>
       <c r="J20" s="21"/>
       <c r="P20" s="9"/>
       <c r="Q20" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>C20+D20+E20+F20+G20+H20+I20+J20+K20+L20+M20+N20+O20+P20</f>
+        <v>1</v>
       </c>
       <c r="R20" s="10"/>
       <c r="S20" s="11"/>
     </row>
     <row r="21" spans="2:19">
-      <c r="B21" s="3"/>
+      <c r="B21" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="C21" s="8"/>
+      <c r="D21" t="b">
+        <v>1</v>
+      </c>
       <c r="J21" s="21"/>
       <c r="P21" s="9"/>
       <c r="Q21" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21+P21</f>
+        <v>1</v>
       </c>
       <c r="R21" s="10"/>
       <c r="S21" s="11"/>
     </row>
     <row r="22" spans="2:19">
-      <c r="B22" s="3"/>
-      <c r="C22" s="8"/>
+      <c r="B22" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="8" t="b">
+        <v>1</v>
+      </c>
       <c r="J22" s="21"/>
       <c r="P22" s="9"/>
       <c r="Q22" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R22" s="10"/>
-      <c r="S22" s="11"/>
+        <f>C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22+P22</f>
+        <v>1</v>
+      </c>
+      <c r="R22" s="12"/>
+      <c r="S22" s="13"/>
     </row>
     <row r="23" spans="2:19">
-      <c r="B23" s="3"/>
+      <c r="B23" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="C23" s="8"/>
+      <c r="D23" t="b">
+        <v>1</v>
+      </c>
       <c r="J23" s="21"/>
       <c r="P23" s="9"/>
       <c r="Q23" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>C23+D23+E23+F23+G23+H23+I23+J23+K23+L23+M23+N23+O23+P23</f>
+        <v>1</v>
       </c>
       <c r="R23" s="10"/>
       <c r="S23" s="11"/>
     </row>
     <row r="24" spans="2:19">
-      <c r="B24" s="3"/>
+      <c r="B24" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="C24" s="8"/>
+      <c r="D24" t="b">
+        <v>1</v>
+      </c>
       <c r="J24" s="21"/>
       <c r="P24" s="9"/>
       <c r="Q24" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>C24+D24+E24+F24+G24+H24+I24+J24+K24+L24+M24+N24+O24+P24</f>
+        <v>1</v>
       </c>
       <c r="R24" s="10"/>
       <c r="S24" s="11"/>
     </row>
     <row r="25" spans="2:19">
-      <c r="B25" s="3"/>
+      <c r="B25" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="C25" s="8"/>
+      <c r="D25" t="b">
+        <v>1</v>
+      </c>
       <c r="J25" s="21"/>
       <c r="P25" s="9"/>
       <c r="Q25" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>C25+D25+E25+F25+G25+H25+I25+J25+K25+L25+M25+N25+O25+P25</f>
+        <v>1</v>
       </c>
       <c r="R25" s="10"/>
       <c r="S25" s="11"/>
     </row>
     <row r="26" spans="2:19">
-      <c r="B26" s="29"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21"/>
+      <c r="B26" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D26" t="b">
+        <v>1</v>
+      </c>
       <c r="J26" s="21"/>
-      <c r="K26" s="21"/>
-      <c r="L26" s="21"/>
-      <c r="M26" s="21"/>
-      <c r="N26" s="21"/>
-      <c r="O26" s="21"/>
-      <c r="P26" s="24"/>
+      <c r="P26" s="9"/>
       <c r="Q26" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R26" s="26"/>
-      <c r="S26" s="34"/>
+        <f>C26+D26+E26+F26+G26+H26+I26+J26+K26+L26+M26+N26+O26+P26</f>
+        <v>2</v>
+      </c>
+      <c r="R26" s="10"/>
+      <c r="S26" s="11"/>
     </row>
     <row r="27" spans="2:19">
       <c r="B27" s="3"/>
@@ -1193,7 +1302,7 @@
       <c r="J27" s="21"/>
       <c r="P27" s="9"/>
       <c r="Q27" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="Q15:Q57" si="1">C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27+P27</f>
         <v>0</v>
       </c>
       <c r="R27" s="10"/>
@@ -1205,7 +1314,7 @@
       <c r="J28" s="21"/>
       <c r="P28" s="9"/>
       <c r="Q28" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R28" s="10"/>
@@ -1217,7 +1326,7 @@
       <c r="J29" s="21"/>
       <c r="P29" s="9"/>
       <c r="Q29" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R29" s="10"/>
@@ -1229,7 +1338,7 @@
       <c r="J30" s="21"/>
       <c r="P30" s="9"/>
       <c r="Q30" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R30" s="10"/>
@@ -1241,7 +1350,7 @@
       <c r="J31" s="21"/>
       <c r="P31" s="9"/>
       <c r="Q31" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R31" s="10"/>
@@ -1253,7 +1362,7 @@
       <c r="J32" s="21"/>
       <c r="P32" s="9"/>
       <c r="Q32" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R32" s="12"/>
@@ -1265,7 +1374,7 @@
       <c r="J33" s="21"/>
       <c r="P33" s="9"/>
       <c r="Q33" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R33" s="10"/>
@@ -1277,7 +1386,7 @@
       <c r="J34" s="21"/>
       <c r="P34" s="9"/>
       <c r="Q34" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R34" s="10"/>
@@ -1300,7 +1409,7 @@
       <c r="O35" s="21"/>
       <c r="P35" s="24"/>
       <c r="Q35" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R35" s="26"/>
@@ -1312,7 +1421,7 @@
       <c r="J36" s="21"/>
       <c r="P36" s="9"/>
       <c r="Q36" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R36" s="10"/>
@@ -1324,7 +1433,7 @@
       <c r="J37" s="21"/>
       <c r="P37" s="9"/>
       <c r="Q37" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R37" s="10"/>
@@ -1336,7 +1445,7 @@
       <c r="J38" s="21"/>
       <c r="P38" s="9"/>
       <c r="Q38" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R38" s="10"/>
@@ -1348,7 +1457,7 @@
       <c r="J39" s="21"/>
       <c r="P39" s="9"/>
       <c r="Q39" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R39" s="10"/>
@@ -1360,7 +1469,7 @@
       <c r="J40" s="21"/>
       <c r="P40" s="9"/>
       <c r="Q40" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R40" s="10"/>
@@ -1372,7 +1481,7 @@
       <c r="J41" s="21"/>
       <c r="P41" s="9"/>
       <c r="Q41" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R41" s="10"/>
@@ -1395,7 +1504,7 @@
       <c r="O42" s="21"/>
       <c r="P42" s="24"/>
       <c r="Q42" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R42" s="26"/>
@@ -1407,7 +1516,7 @@
       <c r="J43" s="21"/>
       <c r="P43" s="9"/>
       <c r="Q43" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R43" s="10"/>
@@ -1419,7 +1528,7 @@
       <c r="J44" s="21"/>
       <c r="P44" s="9"/>
       <c r="Q44" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R44" s="10"/>
@@ -1442,7 +1551,7 @@
       <c r="O45" s="21"/>
       <c r="P45" s="24"/>
       <c r="Q45" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R45" s="28"/>
@@ -1454,7 +1563,7 @@
       <c r="J46" s="21"/>
       <c r="P46" s="9"/>
       <c r="Q46" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R46" s="10"/>
@@ -1466,7 +1575,7 @@
       <c r="J47" s="21"/>
       <c r="P47" s="9"/>
       <c r="Q47" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R47" s="10"/>
@@ -1478,7 +1587,7 @@
       <c r="J48" s="21"/>
       <c r="P48" s="9"/>
       <c r="Q48" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R48" s="12"/>
@@ -1490,7 +1599,7 @@
       <c r="J49" s="21"/>
       <c r="P49" s="9"/>
       <c r="Q49" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R49" s="10"/>
@@ -1502,7 +1611,7 @@
       <c r="J50" s="21"/>
       <c r="P50" s="9"/>
       <c r="Q50" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R50" s="10"/>
@@ -1514,7 +1623,7 @@
       <c r="J51" s="21"/>
       <c r="P51" s="9"/>
       <c r="Q51" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R51" s="10"/>
@@ -1526,7 +1635,7 @@
       <c r="J52" s="21"/>
       <c r="P52" s="9"/>
       <c r="Q52" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R52" s="10"/>
@@ -1538,7 +1647,7 @@
       <c r="J53" s="21"/>
       <c r="P53" s="9"/>
       <c r="Q53" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R53" s="10"/>
@@ -1550,7 +1659,7 @@
       <c r="J54" s="21"/>
       <c r="P54" s="9"/>
       <c r="Q54" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R54" s="10"/>
@@ -1562,7 +1671,7 @@
       <c r="J55" s="21"/>
       <c r="P55" s="9"/>
       <c r="Q55" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R55" s="10"/>
@@ -1574,7 +1683,7 @@
       <c r="J56" s="21"/>
       <c r="P56" s="9"/>
       <c r="Q56" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R56" s="10"/>
@@ -1597,15 +1706,15 @@
       <c r="O57" s="15"/>
       <c r="P57" s="16"/>
       <c r="Q57" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R57" s="17"/>
       <c r="S57" s="18"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S14">
-    <sortCondition ref="B3:B14"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B9:S26">
+    <sortCondition ref="B9:B26"/>
   </sortState>
   <conditionalFormatting sqref="Q3:Q57">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
@@ -1613,5 +1722,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
am adaugat iconite, skills component
</commit_message>
<xml_diff>
--- a/MetodeAvansateDeProgramare/Prezenta_AnII_2024.xlsx
+++ b/MetodeAvansateDeProgramare/Prezenta_AnII_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_Promotia_2023_2026\MetodeAvansateDeProgramare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C367B5-AE1E-45B7-9E4C-B4E354F1A0EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{203CE5E9-0249-4A78-82D5-0497193D1382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>Proiect</t>
   </si>
@@ -138,9 +138,6 @@
     <t>Renata Tirban</t>
   </si>
   <si>
-    <t>AnaMaria  Bohar</t>
-  </si>
-  <si>
     <t>Cristina Nemcea</t>
   </si>
   <si>
@@ -205,6 +202,12 @@
   </si>
   <si>
     <t>Gabriela Maghear</t>
+  </si>
+  <si>
+    <t>Anamaria  Bohar</t>
+  </si>
+  <si>
+    <t>Vlad Brata</t>
   </si>
 </sst>
 </file>
@@ -839,7 +842,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="R7" sqref="R7"/>
+      <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -909,7 +912,7 @@
     </row>
     <row r="3" spans="2:19">
       <c r="B3" s="26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" s="33"/>
       <c r="D3" s="19"/>
@@ -930,7 +933,7 @@
       <c r="O3" s="19"/>
       <c r="P3" s="34"/>
       <c r="Q3" s="4">
-        <f>C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
+        <f t="shared" ref="Q3:Q44" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
         <v>2</v>
       </c>
       <c r="R3" s="35"/>
@@ -949,28 +952,34 @@
       <c r="E4" t="b">
         <v>1</v>
       </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
       <c r="J4" s="18"/>
       <c r="P4" s="6"/>
       <c r="Q4" s="4">
-        <f>C4+D4+E4+F4+G4+H4+I4+J4+K4+L4+M4+N4+O4+P4</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="R4" s="9"/>
       <c r="S4" s="10"/>
     </row>
     <row r="5" spans="2:19">
       <c r="B5" s="3" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" t="b">
         <v>1</v>
       </c>
       <c r="J5" s="18"/>
       <c r="P5" s="6"/>
       <c r="Q5" s="4">
-        <f>C5+D5+E5+F5+G5+H5+I5+J5+K5+L5+M5+N5+O5+P5</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="R5" s="7"/>
       <c r="S5" s="8"/>
@@ -985,7 +994,7 @@
       <c r="J6" s="18"/>
       <c r="P6" s="6"/>
       <c r="Q6" s="4">
-        <f>C6+D6+E6+F6+G6+H6+I6+J6+K6+L6+M6+N6+O6+P6</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R6" s="7"/>
@@ -993,7 +1002,7 @@
     </row>
     <row r="7" spans="2:19">
       <c r="B7" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" s="5"/>
       <c r="E7" t="b">
@@ -1002,7 +1011,7 @@
       <c r="J7" s="18"/>
       <c r="P7" s="6"/>
       <c r="Q7" s="4">
-        <f>C7+D7+E7+F7+G7+H7+I7+J7+K7+L7+M7+N7+O7+P7</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R7" s="7"/>
@@ -1019,7 +1028,7 @@
       <c r="J8" s="18"/>
       <c r="P8" s="6"/>
       <c r="Q8" s="4">
-        <f>C8+D8+E8+F8+G8+H8+I8+J8+K8+L8+M8+N8+O8+P8</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R8" s="7"/>
@@ -1027,7 +1036,7 @@
     </row>
     <row r="9" spans="2:19">
       <c r="B9" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" s="5"/>
       <c r="E9" t="b">
@@ -1039,7 +1048,7 @@
       <c r="J9" s="18"/>
       <c r="P9" s="6"/>
       <c r="Q9" s="4">
-        <f>C9+D9+E9+F9+G9+H9+I9+J9+K9+L9+M9+N9+O9+P9</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R9" s="7"/>
@@ -1047,7 +1056,7 @@
     </row>
     <row r="10" spans="2:19">
       <c r="B10" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C10" s="5"/>
       <c r="E10" t="b">
@@ -1056,7 +1065,7 @@
       <c r="J10" s="18"/>
       <c r="P10" s="6"/>
       <c r="Q10" s="4">
-        <f>C10+D10+E10+F10+G10+H10+I10+J10+K10+L10+M10+N10+O10+P10</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R10" s="7"/>
@@ -1064,7 +1073,7 @@
     </row>
     <row r="11" spans="2:19">
       <c r="B11" s="26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C11" s="20"/>
       <c r="D11" s="18"/>
@@ -1085,7 +1094,7 @@
       <c r="O11" s="18"/>
       <c r="P11" s="21"/>
       <c r="Q11" s="4">
-        <f>C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11+P11</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R11" s="23"/>
@@ -1108,7 +1117,7 @@
       <c r="J12" s="18"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="4">
-        <f>C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12+P12</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R12" s="7"/>
@@ -1116,7 +1125,7 @@
     </row>
     <row r="13" spans="2:19">
       <c r="B13" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C13" s="5"/>
       <c r="E13" t="b">
@@ -1125,7 +1134,7 @@
       <c r="J13" s="18"/>
       <c r="P13" s="6"/>
       <c r="Q13" s="4">
-        <f>C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13+P13</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R13" s="7"/>
@@ -1133,7 +1142,7 @@
     </row>
     <row r="14" spans="2:19">
       <c r="B14" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C14" s="5"/>
       <c r="E14" t="b">
@@ -1142,7 +1151,7 @@
       <c r="J14" s="18"/>
       <c r="P14" s="6"/>
       <c r="Q14" s="4">
-        <f>C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14+P14</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R14" s="9"/>
@@ -1150,7 +1159,7 @@
     </row>
     <row r="15" spans="2:19">
       <c r="B15" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" t="b">
@@ -1162,7 +1171,7 @@
       <c r="J15" s="18"/>
       <c r="P15" s="6"/>
       <c r="Q15" s="4">
-        <f>C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15+P15</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R15" s="7"/>
@@ -1170,17 +1179,20 @@
     </row>
     <row r="16" spans="2:19">
       <c r="B16" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C16" s="5"/>
       <c r="E16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F16" t="b">
         <v>1</v>
       </c>
       <c r="J16" s="18"/>
       <c r="P16" s="6"/>
       <c r="Q16" s="4">
-        <f>C16+D16+E16+F16+G16+H16+I16+J16+K16+L16+M16+N16+O16+P16</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="R16" s="7"/>
       <c r="S16" s="8"/>
@@ -1195,7 +1207,7 @@
       <c r="J17" s="18"/>
       <c r="P17" s="6"/>
       <c r="Q17" s="4">
-        <f>C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17+P17</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R17" s="7"/>
@@ -1220,7 +1232,7 @@
       <c r="J18" s="18"/>
       <c r="P18" s="6"/>
       <c r="Q18" s="4">
-        <f>C18+D18+E18+F18+G18+H18+I18+J18+K18+L18+M18+N18+O18+P18</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="R18" s="7"/>
@@ -1228,7 +1240,7 @@
     </row>
     <row r="19" spans="2:19">
       <c r="B19" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" t="b">
@@ -1240,7 +1252,7 @@
       <c r="J19" s="18"/>
       <c r="P19" s="6"/>
       <c r="Q19" s="4">
-        <f>C19+D19+E19+F19+G19+H19+I19+J19+K19+L19+M19+N19+O19+P19</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R19" s="7"/>
@@ -1260,7 +1272,7 @@
       <c r="J20" s="18"/>
       <c r="P20" s="6"/>
       <c r="Q20" s="4">
-        <f>C20+D20+E20+F20+G20+H20+I20+J20+K20+L20+M20+N20+O20+P20</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R20" s="7"/>
@@ -1268,7 +1280,7 @@
     </row>
     <row r="21" spans="2:19">
       <c r="B21" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C21" s="20"/>
       <c r="D21" s="18" t="b">
@@ -1277,7 +1289,9 @@
       <c r="E21" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="F21" s="18"/>
+      <c r="F21" s="18" t="b">
+        <v>1</v>
+      </c>
       <c r="G21" s="18"/>
       <c r="H21" s="18"/>
       <c r="I21" s="18"/>
@@ -1289,15 +1303,15 @@
       <c r="O21" s="18"/>
       <c r="P21" s="21"/>
       <c r="Q21" s="4">
-        <f>C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21+P21</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="R21" s="23"/>
       <c r="S21" s="31"/>
     </row>
     <row r="22" spans="2:19">
       <c r="B22" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C22" s="5"/>
       <c r="E22" t="b">
@@ -1306,7 +1320,7 @@
       <c r="J22" s="18"/>
       <c r="P22" s="6"/>
       <c r="Q22" s="4">
-        <f>C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22+P22</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R22" s="7"/>
@@ -1339,7 +1353,7 @@
       <c r="O23" s="18"/>
       <c r="P23" s="21"/>
       <c r="Q23" s="4">
-        <f>C23+D23+E23+F23+G23+H23+I23+J23+K23+L23+M23+N23+O23+P23</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="R23" s="23"/>
@@ -1347,7 +1361,7 @@
     </row>
     <row r="24" spans="2:19">
       <c r="B24" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C24" s="5"/>
       <c r="E24" t="b">
@@ -1356,7 +1370,7 @@
       <c r="J24" s="18"/>
       <c r="P24" s="6"/>
       <c r="Q24" s="4">
-        <f>C24+D24+E24+F24+G24+H24+I24+J24+K24+L24+M24+N24+O24+P24</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R24" s="7"/>
@@ -1364,7 +1378,7 @@
     </row>
     <row r="25" spans="2:19">
       <c r="B25" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" t="b">
@@ -1379,7 +1393,7 @@
       <c r="J25" s="18"/>
       <c r="P25" s="6"/>
       <c r="Q25" s="4">
-        <f>C25+D25+E25+F25+G25+H25+I25+J25+K25+L25+M25+N25+O25+P25</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R25" s="7"/>
@@ -1399,7 +1413,7 @@
       <c r="J26" s="18"/>
       <c r="P26" s="6"/>
       <c r="Q26" s="4">
-        <f>C26+D26+E26+F26+G26+H26+I26+J26+K26+L26+M26+N26+O26+P26</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R26" s="9"/>
@@ -1419,7 +1433,7 @@
       <c r="J27" s="18"/>
       <c r="P27" s="6"/>
       <c r="Q27" s="4">
-        <f>C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27+P27</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R27" s="7"/>
@@ -1427,7 +1441,7 @@
     </row>
     <row r="28" spans="2:19">
       <c r="B28" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C28" s="5"/>
       <c r="F28" t="b">
@@ -1436,7 +1450,7 @@
       <c r="J28" s="18"/>
       <c r="P28" s="6"/>
       <c r="Q28" s="4">
-        <f>C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28+P28</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R28" s="7"/>
@@ -1456,7 +1470,7 @@
       <c r="J29" s="18"/>
       <c r="P29" s="6"/>
       <c r="Q29" s="4">
-        <f>C29+D29+E29+F29+G29+H29+I29+J29+K29+L29+M29+N29+O29+P29</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R29" s="7"/>
@@ -1464,7 +1478,7 @@
     </row>
     <row r="30" spans="2:19">
       <c r="B30" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C30" s="5"/>
       <c r="E30" t="b">
@@ -1476,7 +1490,7 @@
       <c r="J30" s="18"/>
       <c r="P30" s="6"/>
       <c r="Q30" s="4">
-        <f>C30+D30+E30+F30+G30+H30+I30+J30+K30+L30+M30+N30+O30+P30</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R30" s="7"/>
@@ -1484,17 +1498,20 @@
     </row>
     <row r="31" spans="2:19">
       <c r="B31" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C31" s="5"/>
       <c r="E31" t="b">
+        <v>1</v>
+      </c>
+      <c r="F31" t="b">
         <v>1</v>
       </c>
       <c r="J31" s="18"/>
       <c r="P31" s="6"/>
       <c r="Q31" s="4">
-        <f>C31+D31+E31+F31+G31+H31+I31+J31+K31+L31+M31+N31+O31+P31</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="R31" s="7"/>
       <c r="S31" s="8"/>
@@ -1513,7 +1530,7 @@
       <c r="J32" s="18"/>
       <c r="P32" s="6"/>
       <c r="Q32" s="4">
-        <f>C32+D32+E32+F32+G32+H32+I32+J32+K32+L32+M32+N32+O32+P32</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R32" s="9"/>
@@ -1521,7 +1538,7 @@
     </row>
     <row r="33" spans="2:19">
       <c r="B33" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C33" s="5"/>
       <c r="E33" t="b">
@@ -1530,7 +1547,7 @@
       <c r="J33" s="18"/>
       <c r="P33" s="6"/>
       <c r="Q33" s="4">
-        <f>C33+D33+E33+F33+G33+H33+I33+J33+K33+L33+M33+N33+O33+P33</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R33" s="7"/>
@@ -1538,7 +1555,7 @@
     </row>
     <row r="34" spans="2:19">
       <c r="B34" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C34" s="5"/>
       <c r="E34" t="b">
@@ -1550,7 +1567,7 @@
       <c r="J34" s="18"/>
       <c r="P34" s="6"/>
       <c r="Q34" s="4">
-        <f>C34+D34+E34+F34+G34+H34+I34+J34+K34+L34+M34+N34+O34+P34</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R34" s="7"/>
@@ -1558,17 +1575,20 @@
     </row>
     <row r="35" spans="2:19">
       <c r="B35" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C35" s="5"/>
       <c r="E35" t="b">
+        <v>1</v>
+      </c>
+      <c r="F35" t="b">
         <v>1</v>
       </c>
       <c r="J35" s="18"/>
       <c r="P35" s="6"/>
       <c r="Q35" s="4">
-        <f>C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="R35" s="7"/>
       <c r="S35" s="8"/>
@@ -1583,11 +1603,14 @@
       <c r="E36" t="b">
         <v>1</v>
       </c>
+      <c r="F36" t="b">
+        <v>1</v>
+      </c>
       <c r="J36" s="18"/>
       <c r="P36" s="6"/>
       <c r="Q36" s="4">
-        <f>C36+D36+E36+F36+G36+H36+I36+J36+K36+L36+M36+N36+O36+P36</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="R36" s="7"/>
       <c r="S36" s="8"/>
@@ -1609,7 +1632,7 @@
       <c r="J37" s="18"/>
       <c r="P37" s="6"/>
       <c r="Q37" s="4">
-        <f>C37+D37+E37+F37+G37+H37+I37+J37+K37+L37+M37+N37+O37+P37</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R37" s="7"/>
@@ -1628,7 +1651,7 @@
       <c r="J38" s="18"/>
       <c r="P38" s="6"/>
       <c r="Q38" s="4">
-        <f>C38+D38+E38+F38+G38+H38+I38+J38+K38+L38+M38+N38+O38+P38</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R38" s="9"/>
@@ -1636,7 +1659,7 @@
     </row>
     <row r="39" spans="2:19">
       <c r="B39" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C39" s="5"/>
       <c r="E39" t="b">
@@ -1648,7 +1671,7 @@
       <c r="J39" s="18"/>
       <c r="P39" s="6"/>
       <c r="Q39" s="4">
-        <f>C39+D39+E39+F39+G39+H39+I39+J39+K39+L39+M39+N39+O39+P39</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R39" s="7"/>
@@ -1665,11 +1688,14 @@
       <c r="E40" t="b">
         <v>1</v>
       </c>
+      <c r="F40" t="b">
+        <v>1</v>
+      </c>
       <c r="J40" s="18"/>
       <c r="P40" s="6"/>
       <c r="Q40" s="4">
-        <f>C40+D40+E40+F40+G40+H40+I40+J40+K40+L40+M40+N40+O40+P40</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="R40" s="7"/>
       <c r="S40" s="8"/>
@@ -1685,18 +1711,21 @@
       <c r="E41" t="b">
         <v>1</v>
       </c>
+      <c r="F41" t="b">
+        <v>1</v>
+      </c>
       <c r="J41" s="18"/>
       <c r="P41" s="6"/>
       <c r="Q41" s="4">
-        <f>C41+D41+E41+F41+G41+H41+I41+J41+K41+L41+M41+N41+O41+P41</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="R41" s="7"/>
       <c r="S41" s="8"/>
     </row>
     <row r="42" spans="2:19">
       <c r="B42" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C42" s="5"/>
       <c r="E42" t="b">
@@ -1708,7 +1737,7 @@
       <c r="J42" s="18"/>
       <c r="P42" s="6"/>
       <c r="Q42" s="4">
-        <f>C42+D42+E42+F42+G42+H42+I42+J42+K42+L42+M42+N42+O42+P42</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R42" s="7"/>
@@ -1731,7 +1760,7 @@
       <c r="J43" s="18"/>
       <c r="P43" s="6"/>
       <c r="Q43" s="4">
-        <f>C43+D43+E43+F43+G43+H43+I43+J43+K43+L43+M43+N43+O43+P43</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R43" s="7"/>
@@ -1750,21 +1779,28 @@
       <c r="E44" t="b">
         <v>1</v>
       </c>
+      <c r="F44" t="b">
+        <v>1</v>
+      </c>
       <c r="J44" s="18"/>
       <c r="P44" s="6"/>
       <c r="Q44" s="4">
-        <f>C44+D44+E44+F44+G44+H44+I44+J44+K44+L44+M44+N44+O44+P44</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="R44" s="7"/>
       <c r="S44" s="8"/>
     </row>
     <row r="45" spans="2:19">
-      <c r="B45" s="26"/>
+      <c r="B45" s="26" t="s">
+        <v>60</v>
+      </c>
       <c r="C45" s="20"/>
       <c r="D45" s="18"/>
       <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
+      <c r="F45" s="18" t="b">
+        <v>1</v>
+      </c>
       <c r="G45" s="18"/>
       <c r="H45" s="18"/>
       <c r="I45" s="18"/>
@@ -1776,8 +1812,8 @@
       <c r="O45" s="18"/>
       <c r="P45" s="21"/>
       <c r="Q45" s="4">
-        <f t="shared" ref="Q44:Q57" si="0">C45+D45+E45+F45+G45+H45+I45+J45+K45+L45+M45+N45+O45+P45</f>
-        <v>0</v>
+        <f t="shared" ref="Q45:Q57" si="1">C45+D45+E45+F45+G45+H45+I45+J45+K45+L45+M45+N45+O45+P45</f>
+        <v>1</v>
       </c>
       <c r="R45" s="25"/>
       <c r="S45" s="24"/>
@@ -1788,7 +1824,7 @@
       <c r="J46" s="18"/>
       <c r="P46" s="6"/>
       <c r="Q46" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R46" s="7"/>
@@ -1800,7 +1836,7 @@
       <c r="J47" s="18"/>
       <c r="P47" s="6"/>
       <c r="Q47" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R47" s="7"/>
@@ -1812,7 +1848,7 @@
       <c r="J48" s="18"/>
       <c r="P48" s="6"/>
       <c r="Q48" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R48" s="9"/>
@@ -1824,7 +1860,7 @@
       <c r="J49" s="18"/>
       <c r="P49" s="6"/>
       <c r="Q49" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R49" s="7"/>
@@ -1836,7 +1872,7 @@
       <c r="J50" s="18"/>
       <c r="P50" s="6"/>
       <c r="Q50" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R50" s="7"/>
@@ -1848,7 +1884,7 @@
       <c r="J51" s="18"/>
       <c r="P51" s="6"/>
       <c r="Q51" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R51" s="7"/>
@@ -1860,7 +1896,7 @@
       <c r="J52" s="18"/>
       <c r="P52" s="6"/>
       <c r="Q52" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R52" s="7"/>
@@ -1872,7 +1908,7 @@
       <c r="J53" s="18"/>
       <c r="P53" s="6"/>
       <c r="Q53" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R53" s="7"/>
@@ -1884,7 +1920,7 @@
       <c r="J54" s="18"/>
       <c r="P54" s="6"/>
       <c r="Q54" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R54" s="7"/>
@@ -1896,7 +1932,7 @@
       <c r="J55" s="18"/>
       <c r="P55" s="6"/>
       <c r="Q55" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R55" s="7"/>
@@ -1908,7 +1944,7 @@
       <c r="J56" s="18"/>
       <c r="P56" s="6"/>
       <c r="Q56" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R56" s="7"/>
@@ -1931,7 +1967,7 @@
       <c r="O57" s="12"/>
       <c r="P57" s="13"/>
       <c r="Q57" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R57" s="14"/>

</xml_diff>

<commit_message>
am adaugat posibilitatea de a edita detaliile personale
</commit_message>
<xml_diff>
--- a/MetodeAvansateDeProgramare/Prezenta_AnII_2024.xlsx
+++ b/MetodeAvansateDeProgramare/Prezenta_AnII_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_Promotia_2023_2026\MetodeAvansateDeProgramare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{203CE5E9-0249-4A78-82D5-0497193D1382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC5D887-4B8A-438F-B958-5D3439E1F49F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>Proiect</t>
   </si>
@@ -208,6 +208,24 @@
   </si>
   <si>
     <t>Vlad Brata</t>
+  </si>
+  <si>
+    <t>Victor Pitirici</t>
+  </si>
+  <si>
+    <t>Madalin Blaj</t>
+  </si>
+  <si>
+    <t>Daniel Oistic</t>
+  </si>
+  <si>
+    <t>Stefan Tulvan</t>
+  </si>
+  <si>
+    <t>David Florea</t>
+  </si>
+  <si>
+    <t>Raul Vonhala</t>
   </si>
 </sst>
 </file>
@@ -463,7 +481,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -545,6 +563,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -839,10 +860,10 @@
   <dimension ref="B2:S57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomRight" activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -933,7 +954,7 @@
       <c r="O3" s="19"/>
       <c r="P3" s="34"/>
       <c r="Q3" s="4">
-        <f t="shared" ref="Q3:Q44" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
+        <f>C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
         <v>2</v>
       </c>
       <c r="R3" s="35"/>
@@ -955,11 +976,14 @@
       <c r="F4" t="b">
         <v>1</v>
       </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
       <c r="J4" s="18"/>
       <c r="P4" s="6"/>
       <c r="Q4" s="4">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>C4+D4+E4+F4+G4+H4+I4+J4+K4+L4+M4+N4+O4+P4</f>
+        <v>5</v>
       </c>
       <c r="R4" s="9"/>
       <c r="S4" s="10"/>
@@ -975,11 +999,14 @@
       <c r="F5" t="b">
         <v>1</v>
       </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
       <c r="J5" s="18"/>
       <c r="P5" s="6"/>
       <c r="Q5" s="4">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C5+D5+E5+F5+G5+H5+I5+J5+K5+L5+M5+N5+O5+P5</f>
+        <v>3</v>
       </c>
       <c r="R5" s="7"/>
       <c r="S5" s="8"/>
@@ -994,7 +1021,7 @@
       <c r="J6" s="18"/>
       <c r="P6" s="6"/>
       <c r="Q6" s="4">
-        <f t="shared" si="0"/>
+        <f>C6+D6+E6+F6+G6+H6+I6+J6+K6+L6+M6+N6+O6+P6</f>
         <v>1</v>
       </c>
       <c r="R6" s="7"/>
@@ -1011,7 +1038,7 @@
       <c r="J7" s="18"/>
       <c r="P7" s="6"/>
       <c r="Q7" s="4">
-        <f t="shared" si="0"/>
+        <f>C7+D7+E7+F7+G7+H7+I7+J7+K7+L7+M7+N7+O7+P7</f>
         <v>1</v>
       </c>
       <c r="R7" s="7"/>
@@ -1028,7 +1055,7 @@
       <c r="J8" s="18"/>
       <c r="P8" s="6"/>
       <c r="Q8" s="4">
-        <f t="shared" si="0"/>
+        <f>C8+D8+E8+F8+G8+H8+I8+J8+K8+L8+M8+N8+O8+P8</f>
         <v>1</v>
       </c>
       <c r="R8" s="7"/>
@@ -1048,7 +1075,7 @@
       <c r="J9" s="18"/>
       <c r="P9" s="6"/>
       <c r="Q9" s="4">
-        <f t="shared" si="0"/>
+        <f>C9+D9+E9+F9+G9+H9+I9+J9+K9+L9+M9+N9+O9+P9</f>
         <v>2</v>
       </c>
       <c r="R9" s="7"/>
@@ -1065,7 +1092,7 @@
       <c r="J10" s="18"/>
       <c r="P10" s="6"/>
       <c r="Q10" s="4">
-        <f t="shared" si="0"/>
+        <f>C10+D10+E10+F10+G10+H10+I10+J10+K10+L10+M10+N10+O10+P10</f>
         <v>1</v>
       </c>
       <c r="R10" s="7"/>
@@ -1094,7 +1121,7 @@
       <c r="O11" s="18"/>
       <c r="P11" s="21"/>
       <c r="Q11" s="4">
-        <f t="shared" si="0"/>
+        <f>C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11+P11</f>
         <v>2</v>
       </c>
       <c r="R11" s="23"/>
@@ -1117,7 +1144,7 @@
       <c r="J12" s="18"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="4">
-        <f t="shared" si="0"/>
+        <f>C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12+P12</f>
         <v>3</v>
       </c>
       <c r="R12" s="7"/>
@@ -1134,7 +1161,7 @@
       <c r="J13" s="18"/>
       <c r="P13" s="6"/>
       <c r="Q13" s="4">
-        <f t="shared" si="0"/>
+        <f>C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13+P13</f>
         <v>1</v>
       </c>
       <c r="R13" s="7"/>
@@ -1148,11 +1175,14 @@
       <c r="E14" t="b">
         <v>1</v>
       </c>
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
       <c r="J14" s="18"/>
       <c r="P14" s="6"/>
       <c r="Q14" s="4">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14+P14</f>
+        <v>2</v>
       </c>
       <c r="R14" s="9"/>
       <c r="S14" s="10"/>
@@ -1171,7 +1201,7 @@
       <c r="J15" s="18"/>
       <c r="P15" s="6"/>
       <c r="Q15" s="4">
-        <f t="shared" si="0"/>
+        <f>C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15+P15</f>
         <v>2</v>
       </c>
       <c r="R15" s="7"/>
@@ -1188,11 +1218,14 @@
       <c r="F16" t="b">
         <v>1</v>
       </c>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
       <c r="J16" s="18"/>
       <c r="P16" s="6"/>
       <c r="Q16" s="4">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C16+D16+E16+F16+G16+H16+I16+J16+K16+L16+M16+N16+O16+P16</f>
+        <v>3</v>
       </c>
       <c r="R16" s="7"/>
       <c r="S16" s="8"/>
@@ -1207,7 +1240,7 @@
       <c r="J17" s="18"/>
       <c r="P17" s="6"/>
       <c r="Q17" s="4">
-        <f t="shared" si="0"/>
+        <f>C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17+P17</f>
         <v>1</v>
       </c>
       <c r="R17" s="7"/>
@@ -1229,11 +1262,14 @@
       <c r="F18" t="b">
         <v>1</v>
       </c>
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
       <c r="J18" s="18"/>
       <c r="P18" s="6"/>
       <c r="Q18" s="4">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>C18+D18+E18+F18+G18+H18+I18+J18+K18+L18+M18+N18+O18+P18</f>
+        <v>5</v>
       </c>
       <c r="R18" s="7"/>
       <c r="S18" s="8"/>
@@ -1249,336 +1285,350 @@
       <c r="E19" t="b">
         <v>1</v>
       </c>
+      <c r="G19" t="b">
+        <v>1</v>
+      </c>
       <c r="J19" s="18"/>
       <c r="P19" s="6"/>
       <c r="Q19" s="4">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C19+D19+E19+F19+G19+H19+I19+J19+K19+L19+M19+N19+O19+P19</f>
+        <v>3</v>
       </c>
       <c r="R19" s="7"/>
       <c r="S19" s="8"/>
     </row>
     <row r="20" spans="2:19">
       <c r="B20" s="3" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="C20" s="5"/>
-      <c r="D20" t="b">
-        <v>1</v>
-      </c>
-      <c r="E20" t="b">
+      <c r="G20" t="b">
         <v>1</v>
       </c>
       <c r="J20" s="18"/>
       <c r="P20" s="6"/>
       <c r="Q20" s="4">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="R20" s="7"/>
+        <f>C20+D20+E20+F20+G20+H20+I20+J20+K20+L20+M20+N20+O20+P20</f>
+        <v>1</v>
+      </c>
+      <c r="R20" s="9"/>
       <c r="S20" s="8"/>
     </row>
     <row r="21" spans="2:19">
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E21" t="b">
+        <v>1</v>
+      </c>
+      <c r="G21" t="b">
+        <v>1</v>
+      </c>
+      <c r="J21" s="18"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="4">
+        <f>C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21+P21</f>
+        <v>3</v>
+      </c>
+      <c r="R21" s="7"/>
+      <c r="S21" s="8"/>
+    </row>
+    <row r="22" spans="2:19">
+      <c r="B22" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="20"/>
-      <c r="D21" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="E21" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="F21" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="18"/>
-      <c r="L21" s="18"/>
-      <c r="M21" s="18"/>
-      <c r="N21" s="18"/>
-      <c r="O21" s="18"/>
-      <c r="P21" s="21"/>
-      <c r="Q21" s="4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="R21" s="23"/>
-      <c r="S21" s="31"/>
-    </row>
-    <row r="22" spans="2:19">
-      <c r="B22" s="3" t="s">
+      <c r="C22" s="20"/>
+      <c r="D22" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="E22" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="F22" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="G22" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="18"/>
+      <c r="P22" s="21"/>
+      <c r="Q22" s="4">
+        <f>C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22+P22</f>
+        <v>4</v>
+      </c>
+      <c r="R22" s="23"/>
+      <c r="S22" s="31"/>
+    </row>
+    <row r="23" spans="2:19">
+      <c r="B23" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="5"/>
-      <c r="E22" t="b">
-        <v>1</v>
-      </c>
-      <c r="J22" s="18"/>
-      <c r="P22" s="6"/>
-      <c r="Q22" s="4">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="R22" s="7"/>
-      <c r="S22" s="8"/>
-    </row>
-    <row r="23" spans="2:19">
-      <c r="B23" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="D23" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="E23" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="F23" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
+      <c r="C23" s="5"/>
+      <c r="E23" t="b">
+        <v>1</v>
+      </c>
       <c r="J23" s="18"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="18"/>
-      <c r="N23" s="18"/>
-      <c r="O23" s="18"/>
-      <c r="P23" s="21"/>
+      <c r="P23" s="6"/>
       <c r="Q23" s="4">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="R23" s="23"/>
-      <c r="S23" s="31"/>
+        <f>C23+D23+E23+F23+G23+H23+I23+J23+K23+L23+M23+N23+O23+P23</f>
+        <v>1</v>
+      </c>
+      <c r="R23" s="7"/>
+      <c r="S23" s="8"/>
     </row>
     <row r="24" spans="2:19">
       <c r="B24" s="3" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="C24" s="5"/>
-      <c r="E24" t="b">
+      <c r="G24" t="b">
         <v>1</v>
       </c>
       <c r="J24" s="18"/>
       <c r="P24" s="6"/>
       <c r="Q24" s="4">
-        <f t="shared" si="0"/>
+        <f>C24+D24+E24+F24+G24+H24+I24+J24+K24+L24+M24+N24+O24+P24</f>
         <v>1</v>
       </c>
       <c r="R24" s="7"/>
       <c r="S24" s="8"/>
     </row>
     <row r="25" spans="2:19">
-      <c r="B25" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" s="5"/>
-      <c r="D25" t="b">
-        <v>1</v>
-      </c>
-      <c r="E25" t="b">
-        <v>1</v>
-      </c>
-      <c r="F25" t="b">
-        <v>1</v>
-      </c>
+      <c r="B25" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D25" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="E25" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="F25" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
       <c r="J25" s="18"/>
-      <c r="P25" s="6"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="18"/>
+      <c r="N25" s="18"/>
+      <c r="O25" s="18"/>
+      <c r="P25" s="21"/>
       <c r="Q25" s="4">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="R25" s="7"/>
-      <c r="S25" s="8"/>
+        <f>C25+D25+E25+F25+G25+H25+I25+J25+K25+L25+M25+N25+O25+P25</f>
+        <v>4</v>
+      </c>
+      <c r="R25" s="23"/>
+      <c r="S25" s="31"/>
     </row>
     <row r="26" spans="2:19">
       <c r="B26" s="3" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C26" s="5"/>
-      <c r="D26" t="b">
-        <v>1</v>
-      </c>
       <c r="E26" t="b">
         <v>1</v>
       </c>
       <c r="J26" s="18"/>
       <c r="P26" s="6"/>
       <c r="Q26" s="4">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="R26" s="9"/>
-      <c r="S26" s="10"/>
+        <f>C26+D26+E26+F26+G26+H26+I26+J26+K26+L26+M26+N26+O26+P26</f>
+        <v>1</v>
+      </c>
+      <c r="R26" s="7"/>
+      <c r="S26" s="8"/>
     </row>
     <row r="27" spans="2:19">
       <c r="B27" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" t="b">
         <v>1</v>
       </c>
       <c r="E27" t="b">
+        <v>1</v>
+      </c>
+      <c r="F27" t="b">
         <v>1</v>
       </c>
       <c r="J27" s="18"/>
       <c r="P27" s="6"/>
       <c r="Q27" s="4">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27+P27</f>
+        <v>3</v>
       </c>
       <c r="R27" s="7"/>
       <c r="S27" s="8"/>
     </row>
     <row r="28" spans="2:19">
       <c r="B28" s="3" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="C28" s="5"/>
-      <c r="F28" t="b">
+      <c r="D28" t="b">
+        <v>1</v>
+      </c>
+      <c r="E28" t="b">
         <v>1</v>
       </c>
       <c r="J28" s="18"/>
       <c r="P28" s="6"/>
       <c r="Q28" s="4">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="R28" s="7"/>
-      <c r="S28" s="8"/>
+        <f>C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28+P28</f>
+        <v>2</v>
+      </c>
+      <c r="R28" s="9"/>
+      <c r="S28" s="10"/>
     </row>
     <row r="29" spans="2:19">
       <c r="B29" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" t="b">
         <v>1</v>
       </c>
       <c r="E29" t="b">
+        <v>1</v>
+      </c>
+      <c r="G29" t="b">
         <v>1</v>
       </c>
       <c r="J29" s="18"/>
       <c r="P29" s="6"/>
       <c r="Q29" s="4">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C29+D29+E29+F29+G29+H29+I29+J29+K29+L29+M29+N29+O29+P29</f>
+        <v>3</v>
       </c>
       <c r="R29" s="7"/>
       <c r="S29" s="8"/>
     </row>
     <row r="30" spans="2:19">
       <c r="B30" s="3" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="C30" s="5"/>
-      <c r="E30" t="b">
-        <v>1</v>
-      </c>
       <c r="F30" t="b">
         <v>1</v>
       </c>
       <c r="J30" s="18"/>
       <c r="P30" s="6"/>
       <c r="Q30" s="4">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C30+D30+E30+F30+G30+H30+I30+J30+K30+L30+M30+N30+O30+P30</f>
+        <v>1</v>
       </c>
       <c r="R30" s="7"/>
       <c r="S30" s="8"/>
     </row>
     <row r="31" spans="2:19">
       <c r="B31" s="3" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C31" s="5"/>
+      <c r="D31" t="b">
+        <v>1</v>
+      </c>
       <c r="E31" t="b">
         <v>1</v>
       </c>
-      <c r="F31" t="b">
+      <c r="G31" t="b">
         <v>1</v>
       </c>
       <c r="J31" s="18"/>
       <c r="P31" s="6"/>
       <c r="Q31" s="4">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C31+D31+E31+F31+G31+H31+I31+J31+K31+L31+M31+N31+O31+P31</f>
+        <v>3</v>
       </c>
       <c r="R31" s="7"/>
       <c r="S31" s="8"/>
     </row>
     <row r="32" spans="2:19">
       <c r="B32" s="3" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="C32" s="5"/>
-      <c r="D32" t="b">
+      <c r="E32" t="b">
         <v>1</v>
       </c>
       <c r="F32" t="b">
+        <v>1</v>
+      </c>
+      <c r="G32" t="b">
         <v>1</v>
       </c>
       <c r="J32" s="18"/>
       <c r="P32" s="6"/>
       <c r="Q32" s="4">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="R32" s="9"/>
-      <c r="S32" s="10"/>
+        <f>C32+D32+E32+F32+G32+H32+I32+J32+K32+L32+M32+N32+O32+P32</f>
+        <v>3</v>
+      </c>
+      <c r="R32" s="7"/>
+      <c r="S32" s="8"/>
     </row>
     <row r="33" spans="2:19">
       <c r="B33" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C33" s="5"/>
       <c r="E33" t="b">
+        <v>1</v>
+      </c>
+      <c r="F33" t="b">
+        <v>1</v>
+      </c>
+      <c r="G33" t="b">
         <v>1</v>
       </c>
       <c r="J33" s="18"/>
       <c r="P33" s="6"/>
       <c r="Q33" s="4">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>C33+D33+E33+F33+G33+H33+I33+J33+K33+L33+M33+N33+O33+P33</f>
+        <v>3</v>
       </c>
       <c r="R33" s="7"/>
       <c r="S33" s="8"/>
     </row>
     <row r="34" spans="2:19">
       <c r="B34" s="3" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="C34" s="5"/>
-      <c r="E34" t="b">
-        <v>1</v>
-      </c>
-      <c r="F34" t="b">
+      <c r="G34" t="b">
         <v>1</v>
       </c>
       <c r="J34" s="18"/>
       <c r="P34" s="6"/>
       <c r="Q34" s="4">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C34+D34+E34+F34+G34+H34+I34+J34+K34+L34+M34+N34+O34+P34</f>
+        <v>1</v>
       </c>
       <c r="R34" s="7"/>
       <c r="S34" s="8"/>
     </row>
     <row r="35" spans="2:19">
       <c r="B35" s="3" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="C35" s="5"/>
-      <c r="E35" t="b">
+      <c r="D35" t="b">
         <v>1</v>
       </c>
       <c r="F35" t="b">
@@ -1587,42 +1637,37 @@
       <c r="J35" s="18"/>
       <c r="P35" s="6"/>
       <c r="Q35" s="4">
-        <f t="shared" si="0"/>
+        <f>C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
         <v>2</v>
       </c>
-      <c r="R35" s="7"/>
-      <c r="S35" s="8"/>
+      <c r="R35" s="9"/>
+      <c r="S35" s="10"/>
     </row>
     <row r="36" spans="2:19">
       <c r="B36" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C36" s="5" t="b">
-        <v>1</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="C36" s="5"/>
       <c r="E36" t="b">
         <v>1</v>
       </c>
-      <c r="F36" t="b">
+      <c r="G36" t="b">
         <v>1</v>
       </c>
       <c r="J36" s="18"/>
       <c r="P36" s="6"/>
       <c r="Q36" s="4">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>C36+D36+E36+F36+G36+H36+I36+J36+K36+L36+M36+N36+O36+P36</f>
+        <v>2</v>
       </c>
       <c r="R36" s="7"/>
       <c r="S36" s="8"/>
     </row>
     <row r="37" spans="2:19">
       <c r="B37" s="3" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="C37" s="5"/>
-      <c r="D37" t="b">
-        <v>1</v>
-      </c>
       <c r="E37" t="b">
         <v>1</v>
       </c>
@@ -1632,54 +1677,63 @@
       <c r="J37" s="18"/>
       <c r="P37" s="6"/>
       <c r="Q37" s="4">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>C37+D37+E37+F37+G37+H37+I37+J37+K37+L37+M37+N37+O37+P37</f>
+        <v>2</v>
       </c>
       <c r="R37" s="7"/>
       <c r="S37" s="8"/>
     </row>
     <row r="38" spans="2:19">
       <c r="B38" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C38" s="5" t="b">
+        <v>57</v>
+      </c>
+      <c r="C38" s="5"/>
+      <c r="E38" t="b">
         <v>1</v>
       </c>
       <c r="F38" t="b">
+        <v>1</v>
+      </c>
+      <c r="G38" t="b">
         <v>1</v>
       </c>
       <c r="J38" s="18"/>
       <c r="P38" s="6"/>
       <c r="Q38" s="4">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="R38" s="9"/>
-      <c r="S38" s="10"/>
+        <f>C38+D38+E38+F38+G38+H38+I38+J38+K38+L38+M38+N38+O38+P38</f>
+        <v>3</v>
+      </c>
+      <c r="R38" s="7"/>
+      <c r="S38" s="8"/>
     </row>
     <row r="39" spans="2:19">
       <c r="B39" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C39" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="C39" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="E39" t="b">
         <v>1</v>
       </c>
       <c r="F39" t="b">
+        <v>1</v>
+      </c>
+      <c r="G39" t="b">
         <v>1</v>
       </c>
       <c r="J39" s="18"/>
       <c r="P39" s="6"/>
       <c r="Q39" s="4">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>C39+D39+E39+F39+G39+H39+I39+J39+K39+L39+M39+N39+O39+P39</f>
+        <v>4</v>
       </c>
       <c r="R39" s="7"/>
       <c r="S39" s="8"/>
     </row>
     <row r="40" spans="2:19">
       <c r="B40" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" t="b">
@@ -1694,7 +1748,7 @@
       <c r="J40" s="18"/>
       <c r="P40" s="6"/>
       <c r="Q40" s="4">
-        <f t="shared" si="0"/>
+        <f>C40+D40+E40+F40+G40+H40+I40+J40+K40+L40+M40+N40+O40+P40</f>
         <v>3</v>
       </c>
       <c r="R40" s="7"/>
@@ -1702,65 +1756,61 @@
     </row>
     <row r="41" spans="2:19">
       <c r="B41" s="3" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="C41" s="5"/>
-      <c r="D41" t="b">
-        <v>1</v>
-      </c>
-      <c r="E41" t="b">
-        <v>1</v>
-      </c>
-      <c r="F41" t="b">
+      <c r="G41" t="b">
         <v>1</v>
       </c>
       <c r="J41" s="18"/>
       <c r="P41" s="6"/>
       <c r="Q41" s="4">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>C41+D41+E41+F41+G41+H41+I41+J41+K41+L41+M41+N41+O41+P41</f>
+        <v>1</v>
       </c>
       <c r="R41" s="7"/>
       <c r="S41" s="8"/>
     </row>
     <row r="42" spans="2:19">
       <c r="B42" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C42" s="5"/>
-      <c r="E42" t="b">
+        <v>22</v>
+      </c>
+      <c r="C42" s="5" t="b">
         <v>1</v>
       </c>
       <c r="F42" t="b">
+        <v>1</v>
+      </c>
+      <c r="G42" t="b">
         <v>1</v>
       </c>
       <c r="J42" s="18"/>
       <c r="P42" s="6"/>
       <c r="Q42" s="4">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="R42" s="7"/>
-      <c r="S42" s="8"/>
+        <f>C42+D42+E42+F42+G42+H42+I42+J42+K42+L42+M42+N42+O42+P42</f>
+        <v>3</v>
+      </c>
+      <c r="R42" s="9"/>
+      <c r="S42" s="10"/>
     </row>
     <row r="43" spans="2:19">
       <c r="B43" s="3" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="C43" s="5"/>
-      <c r="D43" t="b">
-        <v>1</v>
-      </c>
       <c r="E43" t="b">
         <v>1</v>
       </c>
       <c r="F43" t="b">
+        <v>1</v>
+      </c>
+      <c r="G43" t="b">
         <v>1</v>
       </c>
       <c r="J43" s="18"/>
       <c r="P43" s="6"/>
       <c r="Q43" s="4">
-        <f t="shared" si="0"/>
+        <f>C43+D43+E43+F43+G43+H43+I43+J43+K43+L43+M43+N43+O43+P43</f>
         <v>3</v>
       </c>
       <c r="R43" s="7"/>
@@ -1768,11 +1818,9 @@
     </row>
     <row r="44" spans="2:19">
       <c r="B44" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="C44" s="5" t="b">
-        <v>1</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="C44" s="5"/>
       <c r="D44" t="b">
         <v>1</v>
       </c>
@@ -1780,112 +1828,173 @@
         <v>1</v>
       </c>
       <c r="F44" t="b">
+        <v>1</v>
+      </c>
+      <c r="G44" t="b">
         <v>1</v>
       </c>
       <c r="J44" s="18"/>
       <c r="P44" s="6"/>
       <c r="Q44" s="4">
-        <f t="shared" si="0"/>
+        <f>C44+D44+E44+F44+G44+H44+I44+J44+K44+L44+M44+N44+O44+P44</f>
         <v>4</v>
       </c>
       <c r="R44" s="7"/>
       <c r="S44" s="8"/>
     </row>
     <row r="45" spans="2:19">
-      <c r="B45" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="C45" s="20"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="G45" s="18"/>
-      <c r="H45" s="18"/>
-      <c r="I45" s="18"/>
+      <c r="B45" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C45" s="5"/>
+      <c r="D45" t="b">
+        <v>1</v>
+      </c>
+      <c r="E45" t="b">
+        <v>1</v>
+      </c>
+      <c r="F45" t="b">
+        <v>1</v>
+      </c>
+      <c r="G45" t="b">
+        <v>1</v>
+      </c>
       <c r="J45" s="18"/>
-      <c r="K45" s="18"/>
-      <c r="L45" s="18"/>
-      <c r="M45" s="18"/>
-      <c r="N45" s="18"/>
-      <c r="O45" s="18"/>
-      <c r="P45" s="21"/>
+      <c r="P45" s="6"/>
       <c r="Q45" s="4">
-        <f t="shared" ref="Q45:Q57" si="1">C45+D45+E45+F45+G45+H45+I45+J45+K45+L45+M45+N45+O45+P45</f>
-        <v>1</v>
-      </c>
-      <c r="R45" s="25"/>
-      <c r="S45" s="24"/>
+        <f>C45+D45+E45+F45+G45+H45+I45+J45+K45+L45+M45+N45+O45+P45</f>
+        <v>4</v>
+      </c>
+      <c r="R45" s="7"/>
+      <c r="S45" s="8"/>
     </row>
     <row r="46" spans="2:19">
-      <c r="B46" s="3"/>
+      <c r="B46" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="C46" s="5"/>
+      <c r="E46" t="b">
+        <v>1</v>
+      </c>
+      <c r="F46" t="b">
+        <v>1</v>
+      </c>
       <c r="J46" s="18"/>
       <c r="P46" s="6"/>
       <c r="Q46" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>C46+D46+E46+F46+G46+H46+I46+J46+K46+L46+M46+N46+O46+P46</f>
+        <v>2</v>
       </c>
       <c r="R46" s="7"/>
       <c r="S46" s="8"/>
     </row>
     <row r="47" spans="2:19">
-      <c r="B47" s="3"/>
+      <c r="B47" s="3" t="s">
+        <v>64</v>
+      </c>
       <c r="C47" s="5"/>
+      <c r="G47" t="b">
+        <v>1</v>
+      </c>
       <c r="J47" s="18"/>
       <c r="P47" s="6"/>
       <c r="Q47" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>C47+D47+E47+F47+G47+H47+I47+J47+K47+L47+M47+N47+O47+P47</f>
+        <v>1</v>
       </c>
       <c r="R47" s="7"/>
       <c r="S47" s="8"/>
     </row>
     <row r="48" spans="2:19">
-      <c r="B48" s="3"/>
+      <c r="B48" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="C48" s="5"/>
+      <c r="D48" t="b">
+        <v>1</v>
+      </c>
+      <c r="E48" t="b">
+        <v>1</v>
+      </c>
+      <c r="F48" t="b">
+        <v>1</v>
+      </c>
       <c r="J48" s="18"/>
       <c r="P48" s="6"/>
       <c r="Q48" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R48" s="9"/>
+        <f>C48+D48+E48+F48+G48+H48+I48+J48+K48+L48+M48+N48+O48+P48</f>
+        <v>3</v>
+      </c>
+      <c r="R48" s="7"/>
       <c r="S48" s="8"/>
     </row>
     <row r="49" spans="2:19">
-      <c r="B49" s="27"/>
+      <c r="B49" s="27" t="s">
+        <v>61</v>
+      </c>
       <c r="C49" s="5"/>
+      <c r="G49" t="b">
+        <v>1</v>
+      </c>
       <c r="J49" s="18"/>
       <c r="P49" s="6"/>
       <c r="Q49" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>C49+D49+E49+F49+G49+H49+I49+J49+K49+L49+M49+N49+O49+P49</f>
+        <v>1</v>
       </c>
       <c r="R49" s="7"/>
       <c r="S49" s="8"/>
     </row>
     <row r="50" spans="2:19">
-      <c r="B50" s="27"/>
-      <c r="C50" s="5"/>
+      <c r="B50" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="C50" s="20"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="G50" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="H50" s="18"/>
+      <c r="I50" s="18"/>
       <c r="J50" s="18"/>
-      <c r="P50" s="6"/>
+      <c r="K50" s="18"/>
+      <c r="L50" s="18"/>
+      <c r="M50" s="18"/>
+      <c r="N50" s="18"/>
+      <c r="O50" s="18"/>
+      <c r="P50" s="21"/>
       <c r="Q50" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R50" s="7"/>
-      <c r="S50" s="8"/>
+        <f>C50+D50+E50+F50+G50+H50+I50+J50+K50+L50+M50+N50+O50+P50</f>
+        <v>2</v>
+      </c>
+      <c r="R50" s="25"/>
+      <c r="S50" s="24"/>
     </row>
     <row r="51" spans="2:19">
-      <c r="B51" s="27"/>
-      <c r="C51" s="5"/>
+      <c r="B51" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C51" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D51" t="b">
+        <v>1</v>
+      </c>
+      <c r="E51" t="b">
+        <v>1</v>
+      </c>
+      <c r="F51" t="b">
+        <v>1</v>
+      </c>
       <c r="J51" s="18"/>
       <c r="P51" s="6"/>
       <c r="Q51" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>C51+D51+E51+F51+G51+H51+I51+J51+K51+L51+M51+N51+O51+P51</f>
+        <v>4</v>
       </c>
       <c r="R51" s="7"/>
       <c r="S51" s="8"/>
@@ -1896,7 +2005,7 @@
       <c r="J52" s="18"/>
       <c r="P52" s="6"/>
       <c r="Q52" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="Q48:Q57" si="0">C52+D52+E52+F52+G52+H52+I52+J52+K52+L52+M52+N52+O52+P52</f>
         <v>0</v>
       </c>
       <c r="R52" s="7"/>
@@ -1908,7 +2017,7 @@
       <c r="J53" s="18"/>
       <c r="P53" s="6"/>
       <c r="Q53" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R53" s="7"/>
@@ -1920,7 +2029,7 @@
       <c r="J54" s="18"/>
       <c r="P54" s="6"/>
       <c r="Q54" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R54" s="7"/>
@@ -1932,7 +2041,7 @@
       <c r="J55" s="18"/>
       <c r="P55" s="6"/>
       <c r="Q55" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R55" s="7"/>
@@ -1944,7 +2053,7 @@
       <c r="J56" s="18"/>
       <c r="P56" s="6"/>
       <c r="Q56" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R56" s="7"/>
@@ -1967,19 +2076,19 @@
       <c r="O57" s="12"/>
       <c r="P57" s="13"/>
       <c r="Q57" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R57" s="14"/>
       <c r="S57" s="15"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S44">
-    <sortCondition ref="B44"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S51">
+    <sortCondition ref="B51"/>
   </sortState>
   <conditionalFormatting sqref="Q3:Q57">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
-      <formula>4</formula>
+      <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
draw graph, colorare harta, componente tare conexe
</commit_message>
<xml_diff>
--- a/MetodeAvansateDeProgramare/Prezenta_AnII_2024.xlsx
+++ b/MetodeAvansateDeProgramare/Prezenta_AnII_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_Promotia_2023_2026\MetodeAvansateDeProgramare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC5D887-4B8A-438F-B958-5D3439E1F49F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F5118F1-E3E1-44FC-898E-A5684127AB35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>Proiect</t>
   </si>
@@ -226,6 +226,18 @@
   </si>
   <si>
     <t>Raul Vonhala</t>
+  </si>
+  <si>
+    <t>Marian Petrita</t>
+  </si>
+  <si>
+    <t>Loris Cioban</t>
+  </si>
+  <si>
+    <t>Kevin Csaba</t>
+  </si>
+  <si>
+    <t>Ana-Maria Preda</t>
   </si>
 </sst>
 </file>
@@ -481,7 +493,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -563,9 +575,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -860,10 +869,10 @@
   <dimension ref="B2:S57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I27" sqref="I27"/>
+      <selection pane="bottomRight" activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1013,9 +1022,10 @@
     </row>
     <row r="6" spans="2:19">
       <c r="B6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="5" t="b">
+        <v>70</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="H6" t="b">
         <v>1</v>
       </c>
       <c r="J6" s="18"/>
@@ -1029,10 +1039,9 @@
     </row>
     <row r="7" spans="2:19">
       <c r="B7" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C7" s="5"/>
-      <c r="E7" t="b">
+        <v>20</v>
+      </c>
+      <c r="C7" s="5" t="b">
         <v>1</v>
       </c>
       <c r="J7" s="18"/>
@@ -1046,10 +1055,10 @@
     </row>
     <row r="8" spans="2:19">
       <c r="B8" s="3" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="C8" s="5"/>
-      <c r="D8" t="b">
+      <c r="E8" t="b">
         <v>1</v>
       </c>
       <c r="J8" s="18"/>
@@ -1063,119 +1072,127 @@
     </row>
     <row r="9" spans="2:19">
       <c r="B9" s="3" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="C9" s="5"/>
-      <c r="E9" t="b">
-        <v>1</v>
-      </c>
-      <c r="F9" t="b">
+      <c r="D9" t="b">
         <v>1</v>
       </c>
       <c r="J9" s="18"/>
       <c r="P9" s="6"/>
       <c r="Q9" s="4">
         <f>C9+D9+E9+F9+G9+H9+I9+J9+K9+L9+M9+N9+O9+P9</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R9" s="7"/>
       <c r="S9" s="8"/>
     </row>
     <row r="10" spans="2:19">
       <c r="B10" s="3" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C10" s="5"/>
       <c r="E10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10" t="b">
         <v>1</v>
       </c>
       <c r="J10" s="18"/>
       <c r="P10" s="6"/>
       <c r="Q10" s="4">
         <f>C10+D10+E10+F10+G10+H10+I10+J10+K10+L10+M10+N10+O10+P10</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R10" s="7"/>
       <c r="S10" s="8"/>
     </row>
     <row r="11" spans="2:19">
-      <c r="B11" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="F11" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
+      <c r="B11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" t="b">
+        <v>1</v>
+      </c>
       <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="18"/>
-      <c r="P11" s="21"/>
+      <c r="P11" s="6"/>
       <c r="Q11" s="4">
         <f>C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11+P11</f>
         <v>2</v>
       </c>
-      <c r="R11" s="23"/>
-      <c r="S11" s="24"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="8"/>
     </row>
     <row r="12" spans="2:19">
-      <c r="B12" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="5"/>
-      <c r="D12" t="b">
-        <v>1</v>
-      </c>
-      <c r="E12" t="b">
-        <v>1</v>
-      </c>
-      <c r="F12" t="b">
-        <v>1</v>
-      </c>
+      <c r="B12" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="20"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" s="18"/>
       <c r="J12" s="18"/>
-      <c r="P12" s="6"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
+      <c r="P12" s="21"/>
       <c r="Q12" s="4">
         <f>C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12+P12</f>
         <v>3</v>
       </c>
-      <c r="R12" s="7"/>
-      <c r="S12" s="8"/>
+      <c r="R12" s="23"/>
+      <c r="S12" s="24"/>
     </row>
     <row r="13" spans="2:19">
       <c r="B13" s="3" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="C13" s="5"/>
+      <c r="D13" t="b">
+        <v>1</v>
+      </c>
       <c r="E13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" t="b">
         <v>1</v>
       </c>
       <c r="J13" s="18"/>
       <c r="P13" s="6"/>
       <c r="Q13" s="4">
         <f>C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13+P13</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R13" s="7"/>
       <c r="S13" s="8"/>
     </row>
     <row r="14" spans="2:19">
       <c r="B14" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C14" s="5"/>
       <c r="E14" t="b">
         <v>1</v>
       </c>
-      <c r="G14" t="b">
+      <c r="H14" t="b">
         <v>1</v>
       </c>
       <c r="J14" s="18"/>
@@ -1184,18 +1201,18 @@
         <f>C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14+P14</f>
         <v>2</v>
       </c>
-      <c r="R14" s="9"/>
-      <c r="S14" s="10"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="8"/>
     </row>
     <row r="15" spans="2:19">
       <c r="B15" s="3" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C15" s="5"/>
-      <c r="D15" t="b">
-        <v>1</v>
-      </c>
       <c r="E15" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15" t="b">
         <v>1</v>
       </c>
       <c r="J15" s="18"/>
@@ -1204,21 +1221,21 @@
         <f>C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15+P15</f>
         <v>2</v>
       </c>
-      <c r="R15" s="7"/>
-      <c r="S15" s="8"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="10"/>
     </row>
     <row r="16" spans="2:19">
       <c r="B16" s="3" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="C16" s="5"/>
+      <c r="D16" t="b">
+        <v>1</v>
+      </c>
       <c r="E16" t="b">
         <v>1</v>
       </c>
-      <c r="F16" t="b">
-        <v>1</v>
-      </c>
-      <c r="G16" t="b">
+      <c r="H16" t="b">
         <v>1</v>
       </c>
       <c r="J16" s="18"/>
@@ -1232,76 +1249,85 @@
     </row>
     <row r="17" spans="2:19">
       <c r="B17" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="5" t="b">
+        <v>54</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="E17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F17" t="b">
+        <v>1</v>
+      </c>
+      <c r="G17" t="b">
         <v>1</v>
       </c>
       <c r="J17" s="18"/>
       <c r="P17" s="6"/>
       <c r="Q17" s="4">
         <f>C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17+P17</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R17" s="7"/>
       <c r="S17" s="8"/>
     </row>
     <row r="18" spans="2:19">
       <c r="B18" s="3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C18" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D18" t="b">
-        <v>1</v>
-      </c>
-      <c r="E18" t="b">
-        <v>1</v>
-      </c>
-      <c r="F18" t="b">
-        <v>1</v>
-      </c>
-      <c r="G18" t="b">
         <v>1</v>
       </c>
       <c r="J18" s="18"/>
       <c r="P18" s="6"/>
       <c r="Q18" s="4">
         <f>C18+D18+E18+F18+G18+H18+I18+J18+K18+L18+M18+N18+O18+P18</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="R18" s="7"/>
       <c r="S18" s="8"/>
     </row>
     <row r="19" spans="2:19">
       <c r="B19" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="C19" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="D19" t="b">
         <v>1</v>
       </c>
       <c r="E19" t="b">
         <v>1</v>
       </c>
+      <c r="F19" t="b">
+        <v>1</v>
+      </c>
       <c r="G19" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19" t="b">
         <v>1</v>
       </c>
       <c r="J19" s="18"/>
       <c r="P19" s="6"/>
       <c r="Q19" s="4">
         <f>C19+D19+E19+F19+G19+H19+I19+J19+K19+L19+M19+N19+O19+P19</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="R19" s="7"/>
       <c r="S19" s="8"/>
     </row>
     <row r="20" spans="2:19">
       <c r="B20" s="3" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="C20" s="5"/>
+      <c r="D20" t="b">
+        <v>1</v>
+      </c>
+      <c r="E20" t="b">
+        <v>1</v>
+      </c>
       <c r="G20" t="b">
         <v>1</v>
       </c>
@@ -1309,22 +1335,16 @@
       <c r="P20" s="6"/>
       <c r="Q20" s="4">
         <f>C20+D20+E20+F20+G20+H20+I20+J20+K20+L20+M20+N20+O20+P20</f>
-        <v>1</v>
-      </c>
-      <c r="R20" s="9"/>
+        <v>3</v>
+      </c>
+      <c r="R20" s="7"/>
       <c r="S20" s="8"/>
     </row>
     <row r="21" spans="2:19">
       <c r="B21" s="3" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="C21" s="5"/>
-      <c r="D21" t="b">
-        <v>1</v>
-      </c>
-      <c r="E21" t="b">
-        <v>1</v>
-      </c>
       <c r="G21" t="b">
         <v>1</v>
       </c>
@@ -1332,243 +1352,249 @@
       <c r="P21" s="6"/>
       <c r="Q21" s="4">
         <f>C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21+P21</f>
-        <v>3</v>
-      </c>
-      <c r="R21" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="R21" s="9"/>
       <c r="S21" s="8"/>
     </row>
     <row r="22" spans="2:19">
-      <c r="B22" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="E22" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="F22" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="G22" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
+      <c r="B22" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" t="b">
+        <v>1</v>
+      </c>
+      <c r="E22" t="b">
+        <v>1</v>
+      </c>
+      <c r="G22" t="b">
+        <v>1</v>
+      </c>
       <c r="J22" s="18"/>
-      <c r="K22" s="18"/>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18"/>
-      <c r="N22" s="18"/>
-      <c r="O22" s="18"/>
-      <c r="P22" s="21"/>
+      <c r="P22" s="6"/>
       <c r="Q22" s="4">
         <f>C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22+P22</f>
-        <v>4</v>
-      </c>
-      <c r="R22" s="23"/>
-      <c r="S22" s="31"/>
+        <v>3</v>
+      </c>
+      <c r="R22" s="7"/>
+      <c r="S22" s="8"/>
     </row>
     <row r="23" spans="2:19">
-      <c r="B23" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" s="5"/>
-      <c r="E23" t="b">
-        <v>1</v>
-      </c>
+      <c r="B23" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="20"/>
+      <c r="D23" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="E23" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="F23" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="G23" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
       <c r="J23" s="18"/>
-      <c r="P23" s="6"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="21"/>
       <c r="Q23" s="4">
         <f>C23+D23+E23+F23+G23+H23+I23+J23+K23+L23+M23+N23+O23+P23</f>
-        <v>1</v>
-      </c>
-      <c r="R23" s="7"/>
-      <c r="S23" s="8"/>
+        <v>4</v>
+      </c>
+      <c r="R23" s="23"/>
+      <c r="S23" s="31"/>
     </row>
     <row r="24" spans="2:19">
       <c r="B24" s="3" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="C24" s="5"/>
-      <c r="G24" t="b">
+      <c r="E24" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24" t="b">
         <v>1</v>
       </c>
       <c r="J24" s="18"/>
       <c r="P24" s="6"/>
       <c r="Q24" s="4">
         <f>C24+D24+E24+F24+G24+H24+I24+J24+K24+L24+M24+N24+O24+P24</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R24" s="7"/>
       <c r="S24" s="8"/>
     </row>
     <row r="25" spans="2:19">
-      <c r="B25" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="D25" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="E25" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="F25" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="G25" s="18"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="18"/>
+      <c r="B25" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="G25" t="b">
+        <v>1</v>
+      </c>
       <c r="J25" s="18"/>
-      <c r="K25" s="18"/>
-      <c r="L25" s="18"/>
-      <c r="M25" s="18"/>
-      <c r="N25" s="18"/>
-      <c r="O25" s="18"/>
-      <c r="P25" s="21"/>
+      <c r="P25" s="6"/>
       <c r="Q25" s="4">
         <f>C25+D25+E25+F25+G25+H25+I25+J25+K25+L25+M25+N25+O25+P25</f>
-        <v>4</v>
-      </c>
-      <c r="R25" s="23"/>
-      <c r="S25" s="31"/>
+        <v>1</v>
+      </c>
+      <c r="R25" s="7"/>
+      <c r="S25" s="8"/>
     </row>
     <row r="26" spans="2:19">
-      <c r="B26" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" s="5"/>
-      <c r="E26" t="b">
-        <v>1</v>
-      </c>
+      <c r="B26" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D26" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="E26" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="F26" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
       <c r="J26" s="18"/>
-      <c r="P26" s="6"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="18"/>
+      <c r="P26" s="21"/>
       <c r="Q26" s="4">
         <f>C26+D26+E26+F26+G26+H26+I26+J26+K26+L26+M26+N26+O26+P26</f>
-        <v>1</v>
-      </c>
-      <c r="R26" s="7"/>
-      <c r="S26" s="8"/>
+        <v>4</v>
+      </c>
+      <c r="R26" s="23"/>
+      <c r="S26" s="31"/>
     </row>
     <row r="27" spans="2:19">
       <c r="B27" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C27" s="5"/>
-      <c r="D27" t="b">
-        <v>1</v>
-      </c>
       <c r="E27" t="b">
         <v>1</v>
       </c>
-      <c r="F27" t="b">
+      <c r="H27" t="b">
         <v>1</v>
       </c>
       <c r="J27" s="18"/>
       <c r="P27" s="6"/>
       <c r="Q27" s="4">
         <f>C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27+P27</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R27" s="7"/>
       <c r="S27" s="8"/>
     </row>
     <row r="28" spans="2:19">
       <c r="B28" s="3" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" t="b">
         <v>1</v>
       </c>
       <c r="E28" t="b">
+        <v>1</v>
+      </c>
+      <c r="F28" t="b">
         <v>1</v>
       </c>
       <c r="J28" s="18"/>
       <c r="P28" s="6"/>
       <c r="Q28" s="4">
         <f>C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28+P28</f>
-        <v>2</v>
-      </c>
-      <c r="R28" s="9"/>
-      <c r="S28" s="10"/>
+        <v>3</v>
+      </c>
+      <c r="R28" s="7"/>
+      <c r="S28" s="8"/>
     </row>
     <row r="29" spans="2:19">
       <c r="B29" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" t="b">
         <v>1</v>
       </c>
       <c r="E29" t="b">
-        <v>1</v>
-      </c>
-      <c r="G29" t="b">
         <v>1</v>
       </c>
       <c r="J29" s="18"/>
       <c r="P29" s="6"/>
       <c r="Q29" s="4">
         <f>C29+D29+E29+F29+G29+H29+I29+J29+K29+L29+M29+N29+O29+P29</f>
-        <v>3</v>
-      </c>
-      <c r="R29" s="7"/>
-      <c r="S29" s="8"/>
+        <v>2</v>
+      </c>
+      <c r="R29" s="9"/>
+      <c r="S29" s="10"/>
     </row>
     <row r="30" spans="2:19">
       <c r="B30" s="3" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="C30" s="5"/>
-      <c r="F30" t="b">
+      <c r="D30" t="b">
+        <v>1</v>
+      </c>
+      <c r="E30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G30" t="b">
         <v>1</v>
       </c>
       <c r="J30" s="18"/>
       <c r="P30" s="6"/>
       <c r="Q30" s="4">
         <f>C30+D30+E30+F30+G30+H30+I30+J30+K30+L30+M30+N30+O30+P30</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R30" s="7"/>
       <c r="S30" s="8"/>
     </row>
     <row r="31" spans="2:19">
       <c r="B31" s="3" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="C31" s="5"/>
-      <c r="D31" t="b">
-        <v>1</v>
-      </c>
-      <c r="E31" t="b">
-        <v>1</v>
-      </c>
-      <c r="G31" t="b">
+      <c r="F31" t="b">
         <v>1</v>
       </c>
       <c r="J31" s="18"/>
       <c r="P31" s="6"/>
       <c r="Q31" s="4">
         <f>C31+D31+E31+F31+G31+H31+I31+J31+K31+L31+M31+N31+O31+P31</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R31" s="7"/>
       <c r="S31" s="8"/>
     </row>
     <row r="32" spans="2:19">
       <c r="B32" s="3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C32" s="5"/>
+      <c r="D32" t="b">
+        <v>1</v>
+      </c>
       <c r="E32" t="b">
-        <v>1</v>
-      </c>
-      <c r="F32" t="b">
         <v>1</v>
       </c>
       <c r="G32" t="b">
@@ -1585,7 +1611,7 @@
     </row>
     <row r="33" spans="2:19">
       <c r="B33" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C33" s="5"/>
       <c r="E33" t="b">
@@ -1595,23 +1621,26 @@
         <v>1</v>
       </c>
       <c r="G33" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33" t="b">
         <v>1</v>
       </c>
       <c r="J33" s="18"/>
       <c r="P33" s="6"/>
       <c r="Q33" s="4">
         <f>C33+D33+E33+F33+G33+H33+I33+J33+K33+L33+M33+N33+O33+P33</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R33" s="7"/>
       <c r="S33" s="8"/>
     </row>
     <row r="34" spans="2:19">
       <c r="B34" s="3" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="C34" s="5"/>
-      <c r="G34" t="b">
+      <c r="H34" t="b">
         <v>1</v>
       </c>
       <c r="J34" s="18"/>
@@ -1625,30 +1654,30 @@
     </row>
     <row r="35" spans="2:19">
       <c r="B35" s="3" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="C35" s="5"/>
-      <c r="D35" t="b">
-        <v>1</v>
-      </c>
-      <c r="F35" t="b">
+      <c r="H35" t="b">
         <v>1</v>
       </c>
       <c r="J35" s="18"/>
       <c r="P35" s="6"/>
       <c r="Q35" s="4">
         <f>C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
-        <v>2</v>
-      </c>
-      <c r="R35" s="9"/>
-      <c r="S35" s="10"/>
+        <v>1</v>
+      </c>
+      <c r="R35" s="7"/>
+      <c r="S35" s="8"/>
     </row>
     <row r="36" spans="2:19">
       <c r="B36" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C36" s="5"/>
       <c r="E36" t="b">
+        <v>1</v>
+      </c>
+      <c r="F36" t="b">
         <v>1</v>
       </c>
       <c r="G36" t="b">
@@ -1658,91 +1687,77 @@
       <c r="P36" s="6"/>
       <c r="Q36" s="4">
         <f>C36+D36+E36+F36+G36+H36+I36+J36+K36+L36+M36+N36+O36+P36</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R36" s="7"/>
       <c r="S36" s="8"/>
     </row>
     <row r="37" spans="2:19">
       <c r="B37" s="3" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="C37" s="5"/>
-      <c r="E37" t="b">
-        <v>1</v>
-      </c>
-      <c r="F37" t="b">
+      <c r="G37" t="b">
         <v>1</v>
       </c>
       <c r="J37" s="18"/>
       <c r="P37" s="6"/>
       <c r="Q37" s="4">
         <f>C37+D37+E37+F37+G37+H37+I37+J37+K37+L37+M37+N37+O37+P37</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R37" s="7"/>
       <c r="S37" s="8"/>
     </row>
     <row r="38" spans="2:19">
       <c r="B38" s="3" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="C38" s="5"/>
-      <c r="E38" t="b">
-        <v>1</v>
-      </c>
-      <c r="F38" t="b">
-        <v>1</v>
-      </c>
-      <c r="G38" t="b">
+      <c r="H38" t="b">
         <v>1</v>
       </c>
       <c r="J38" s="18"/>
       <c r="P38" s="6"/>
       <c r="Q38" s="4">
         <f>C38+D38+E38+F38+G38+H38+I38+J38+K38+L38+M38+N38+O38+P38</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R38" s="7"/>
       <c r="S38" s="8"/>
     </row>
     <row r="39" spans="2:19">
       <c r="B39" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C39" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E39" t="b">
+        <v>30</v>
+      </c>
+      <c r="C39" s="5"/>
+      <c r="D39" t="b">
         <v>1</v>
       </c>
       <c r="F39" t="b">
-        <v>1</v>
-      </c>
-      <c r="G39" t="b">
         <v>1</v>
       </c>
       <c r="J39" s="18"/>
       <c r="P39" s="6"/>
       <c r="Q39" s="4">
         <f>C39+D39+E39+F39+G39+H39+I39+J39+K39+L39+M39+N39+O39+P39</f>
-        <v>4</v>
-      </c>
-      <c r="R39" s="7"/>
-      <c r="S39" s="8"/>
+        <v>2</v>
+      </c>
+      <c r="R39" s="9"/>
+      <c r="S39" s="10"/>
     </row>
     <row r="40" spans="2:19">
       <c r="B40" s="3" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="C40" s="5"/>
-      <c r="D40" t="b">
-        <v>1</v>
-      </c>
       <c r="E40" t="b">
         <v>1</v>
       </c>
-      <c r="F40" t="b">
+      <c r="G40" t="b">
+        <v>1</v>
+      </c>
+      <c r="H40" t="b">
         <v>1</v>
       </c>
       <c r="J40" s="18"/>
@@ -1756,26 +1771,30 @@
     </row>
     <row r="41" spans="2:19">
       <c r="B41" s="3" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="C41" s="5"/>
-      <c r="G41" t="b">
+      <c r="E41" t="b">
+        <v>1</v>
+      </c>
+      <c r="F41" t="b">
         <v>1</v>
       </c>
       <c r="J41" s="18"/>
       <c r="P41" s="6"/>
       <c r="Q41" s="4">
         <f>C41+D41+E41+F41+G41+H41+I41+J41+K41+L41+M41+N41+O41+P41</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R41" s="7"/>
       <c r="S41" s="8"/>
     </row>
     <row r="42" spans="2:19">
       <c r="B42" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C42" s="5" t="b">
+        <v>57</v>
+      </c>
+      <c r="C42" s="5"/>
+      <c r="E42" t="b">
         <v>1</v>
       </c>
       <c r="F42" t="b">
@@ -1790,14 +1809,16 @@
         <f>C42+D42+E42+F42+G42+H42+I42+J42+K42+L42+M42+N42+O42+P42</f>
         <v>3</v>
       </c>
-      <c r="R42" s="9"/>
-      <c r="S42" s="10"/>
+      <c r="R42" s="7"/>
+      <c r="S42" s="8"/>
     </row>
     <row r="43" spans="2:19">
       <c r="B43" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C43" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="C43" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="E43" t="b">
         <v>1</v>
       </c>
@@ -1811,14 +1832,14 @@
       <c r="P43" s="6"/>
       <c r="Q43" s="4">
         <f>C43+D43+E43+F43+G43+H43+I43+J43+K43+L43+M43+N43+O43+P43</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R43" s="7"/>
       <c r="S43" s="8"/>
     </row>
     <row r="44" spans="2:19">
       <c r="B44" s="32" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C44" s="5"/>
       <c r="D44" t="b">
@@ -1828,86 +1849,88 @@
         <v>1</v>
       </c>
       <c r="F44" t="b">
-        <v>1</v>
-      </c>
-      <c r="G44" t="b">
         <v>1</v>
       </c>
       <c r="J44" s="18"/>
       <c r="P44" s="6"/>
       <c r="Q44" s="4">
         <f>C44+D44+E44+F44+G44+H44+I44+J44+K44+L44+M44+N44+O44+P44</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R44" s="7"/>
       <c r="S44" s="8"/>
     </row>
     <row r="45" spans="2:19">
       <c r="B45" s="3" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="C45" s="5"/>
-      <c r="D45" t="b">
-        <v>1</v>
-      </c>
-      <c r="E45" t="b">
-        <v>1</v>
-      </c>
-      <c r="F45" t="b">
-        <v>1</v>
-      </c>
       <c r="G45" t="b">
+        <v>1</v>
+      </c>
+      <c r="H45" t="b">
         <v>1</v>
       </c>
       <c r="J45" s="18"/>
       <c r="P45" s="6"/>
       <c r="Q45" s="4">
         <f>C45+D45+E45+F45+G45+H45+I45+J45+K45+L45+M45+N45+O45+P45</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R45" s="7"/>
       <c r="S45" s="8"/>
     </row>
     <row r="46" spans="2:19">
       <c r="B46" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C46" s="5"/>
-      <c r="E46" t="b">
+        <v>22</v>
+      </c>
+      <c r="C46" s="5" t="b">
         <v>1</v>
       </c>
       <c r="F46" t="b">
+        <v>1</v>
+      </c>
+      <c r="G46" t="b">
         <v>1</v>
       </c>
       <c r="J46" s="18"/>
       <c r="P46" s="6"/>
       <c r="Q46" s="4">
         <f>C46+D46+E46+F46+G46+H46+I46+J46+K46+L46+M46+N46+O46+P46</f>
-        <v>2</v>
-      </c>
-      <c r="R46" s="7"/>
-      <c r="S46" s="8"/>
+        <v>3</v>
+      </c>
+      <c r="R46" s="9"/>
+      <c r="S46" s="10"/>
     </row>
     <row r="47" spans="2:19">
       <c r="B47" s="3" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="C47" s="5"/>
+      <c r="E47" t="b">
+        <v>1</v>
+      </c>
+      <c r="F47" t="b">
+        <v>1</v>
+      </c>
       <c r="G47" t="b">
+        <v>1</v>
+      </c>
+      <c r="H47" t="b">
         <v>1</v>
       </c>
       <c r="J47" s="18"/>
       <c r="P47" s="6"/>
       <c r="Q47" s="4">
         <f>C47+D47+E47+F47+G47+H47+I47+J47+K47+L47+M47+N47+O47+P47</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R47" s="7"/>
       <c r="S47" s="8"/>
     </row>
     <row r="48" spans="2:19">
       <c r="B48" s="3" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="C48" s="5"/>
       <c r="D48" t="b">
@@ -1917,22 +1940,34 @@
         <v>1</v>
       </c>
       <c r="F48" t="b">
+        <v>1</v>
+      </c>
+      <c r="G48" t="b">
         <v>1</v>
       </c>
       <c r="J48" s="18"/>
       <c r="P48" s="6"/>
       <c r="Q48" s="4">
         <f>C48+D48+E48+F48+G48+H48+I48+J48+K48+L48+M48+N48+O48+P48</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R48" s="7"/>
       <c r="S48" s="8"/>
     </row>
     <row r="49" spans="2:19">
       <c r="B49" s="27" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="C49" s="5"/>
+      <c r="D49" t="b">
+        <v>1</v>
+      </c>
+      <c r="E49" t="b">
+        <v>1</v>
+      </c>
+      <c r="F49" t="b">
+        <v>1</v>
+      </c>
       <c r="G49" t="b">
         <v>1</v>
       </c>
@@ -1940,109 +1975,146 @@
       <c r="P49" s="6"/>
       <c r="Q49" s="4">
         <f>C49+D49+E49+F49+G49+H49+I49+J49+K49+L49+M49+N49+O49+P49</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R49" s="7"/>
       <c r="S49" s="8"/>
     </row>
     <row r="50" spans="2:19">
-      <c r="B50" s="37" t="s">
-        <v>60</v>
-      </c>
-      <c r="C50" s="20"/>
-      <c r="D50" s="18"/>
-      <c r="E50" s="18"/>
-      <c r="F50" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="G50" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="H50" s="18"/>
-      <c r="I50" s="18"/>
+      <c r="B50" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="C50" s="5"/>
+      <c r="E50" t="b">
+        <v>1</v>
+      </c>
+      <c r="F50" t="b">
+        <v>1</v>
+      </c>
       <c r="J50" s="18"/>
-      <c r="K50" s="18"/>
-      <c r="L50" s="18"/>
-      <c r="M50" s="18"/>
-      <c r="N50" s="18"/>
-      <c r="O50" s="18"/>
-      <c r="P50" s="21"/>
+      <c r="P50" s="6"/>
       <c r="Q50" s="4">
         <f>C50+D50+E50+F50+G50+H50+I50+J50+K50+L50+M50+N50+O50+P50</f>
         <v>2</v>
       </c>
-      <c r="R50" s="25"/>
-      <c r="S50" s="24"/>
+      <c r="R50" s="7"/>
+      <c r="S50" s="8"/>
     </row>
     <row r="51" spans="2:19">
       <c r="B51" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="C51" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D51" t="b">
-        <v>1</v>
-      </c>
-      <c r="E51" t="b">
-        <v>1</v>
-      </c>
-      <c r="F51" t="b">
+        <v>64</v>
+      </c>
+      <c r="C51" s="5"/>
+      <c r="G51" t="b">
         <v>1</v>
       </c>
       <c r="J51" s="18"/>
       <c r="P51" s="6"/>
       <c r="Q51" s="4">
         <f>C51+D51+E51+F51+G51+H51+I51+J51+K51+L51+M51+N51+O51+P51</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="R51" s="7"/>
       <c r="S51" s="8"/>
     </row>
     <row r="52" spans="2:19">
-      <c r="B52" s="27"/>
+      <c r="B52" s="27" t="s">
+        <v>26</v>
+      </c>
       <c r="C52" s="5"/>
+      <c r="D52" t="b">
+        <v>1</v>
+      </c>
+      <c r="E52" t="b">
+        <v>1</v>
+      </c>
+      <c r="F52" t="b">
+        <v>1</v>
+      </c>
+      <c r="H52" t="b">
+        <v>1</v>
+      </c>
       <c r="J52" s="18"/>
       <c r="P52" s="6"/>
       <c r="Q52" s="4">
-        <f t="shared" ref="Q48:Q57" si="0">C52+D52+E52+F52+G52+H52+I52+J52+K52+L52+M52+N52+O52+P52</f>
-        <v>0</v>
+        <f>C52+D52+E52+F52+G52+H52+I52+J52+K52+L52+M52+N52+O52+P52</f>
+        <v>4</v>
       </c>
       <c r="R52" s="7"/>
       <c r="S52" s="8"/>
     </row>
     <row r="53" spans="2:19">
-      <c r="B53" s="28"/>
+      <c r="B53" s="28" t="s">
+        <v>61</v>
+      </c>
       <c r="C53" s="5"/>
+      <c r="G53" t="b">
+        <v>1</v>
+      </c>
+      <c r="H53" t="b">
+        <v>1</v>
+      </c>
       <c r="J53" s="18"/>
       <c r="P53" s="6"/>
       <c r="Q53" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>C53+D53+E53+F53+G53+H53+I53+J53+K53+L53+M53+N53+O53+P53</f>
+        <v>2</v>
       </c>
       <c r="R53" s="7"/>
       <c r="S53" s="8"/>
     </row>
     <row r="54" spans="2:19">
-      <c r="B54" s="3"/>
-      <c r="C54" s="5"/>
+      <c r="B54" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C54" s="20"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="G54" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="H54" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="I54" s="18"/>
       <c r="J54" s="18"/>
-      <c r="P54" s="6"/>
+      <c r="K54" s="18"/>
+      <c r="L54" s="18"/>
+      <c r="M54" s="18"/>
+      <c r="N54" s="18"/>
+      <c r="O54" s="18"/>
+      <c r="P54" s="21"/>
       <c r="Q54" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R54" s="7"/>
-      <c r="S54" s="8"/>
+        <f>C54+D54+E54+F54+G54+H54+I54+J54+K54+L54+M54+N54+O54+P54</f>
+        <v>3</v>
+      </c>
+      <c r="R54" s="25"/>
+      <c r="S54" s="24"/>
     </row>
     <row r="55" spans="2:19">
-      <c r="B55" s="3"/>
-      <c r="C55" s="5"/>
+      <c r="B55" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C55" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D55" t="b">
+        <v>1</v>
+      </c>
+      <c r="E55" t="b">
+        <v>1</v>
+      </c>
+      <c r="F55" t="b">
+        <v>1</v>
+      </c>
       <c r="J55" s="18"/>
       <c r="P55" s="6"/>
       <c r="Q55" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>C55+D55+E55+F55+G55+H55+I55+J55+K55+L55+M55+N55+O55+P55</f>
+        <v>4</v>
       </c>
       <c r="R55" s="7"/>
       <c r="S55" s="8"/>
@@ -2053,7 +2125,7 @@
       <c r="J56" s="18"/>
       <c r="P56" s="6"/>
       <c r="Q56" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="Q52:Q57" si="0">C56+D56+E56+F56+G56+H56+I56+J56+K56+L56+M56+N56+O56+P56</f>
         <v>0</v>
       </c>
       <c r="R56" s="7"/>
@@ -2083,8 +2155,8 @@
       <c r="S57" s="15"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S51">
-    <sortCondition ref="B51"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S55">
+    <sortCondition ref="B55"/>
   </sortState>
   <conditionalFormatting sqref="Q3:Q57">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">

</xml_diff>

<commit_message>
formular de adaugare al unui skill; rafinare al formularului de la personal details
</commit_message>
<xml_diff>
--- a/MetodeAvansateDeProgramare/Prezenta_AnII_2024.xlsx
+++ b/MetodeAvansateDeProgramare/Prezenta_AnII_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_Promotia_2023_2026\MetodeAvansateDeProgramare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F5118F1-E3E1-44FC-898E-A5684127AB35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61FBD99D-4414-49CC-B3B2-DC847BA5B190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>Proiect</t>
   </si>
@@ -238,6 +238,9 @@
   </si>
   <si>
     <t>Ana-Maria Preda</t>
+  </si>
+  <si>
+    <t>Victor Balaj</t>
   </si>
 </sst>
 </file>
@@ -869,10 +872,10 @@
   <dimension ref="B2:S57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K41" sqref="K41"/>
+      <selection pane="bottomRight" activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -963,7 +966,7 @@
       <c r="O3" s="19"/>
       <c r="P3" s="34"/>
       <c r="Q3" s="4">
-        <f>C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
+        <f t="shared" ref="Q3:Q34" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
         <v>2</v>
       </c>
       <c r="R3" s="35"/>
@@ -988,11 +991,14 @@
       <c r="G4" t="b">
         <v>1</v>
       </c>
+      <c r="H4" t="b">
+        <v>1</v>
+      </c>
       <c r="J4" s="18"/>
       <c r="P4" s="6"/>
       <c r="Q4" s="4">
-        <f>C4+D4+E4+F4+G4+H4+I4+J4+K4+L4+M4+N4+O4+P4</f>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="R4" s="9"/>
       <c r="S4" s="10"/>
@@ -1011,11 +1017,14 @@
       <c r="G5" t="b">
         <v>1</v>
       </c>
+      <c r="H5" t="b">
+        <v>1</v>
+      </c>
       <c r="J5" s="18"/>
       <c r="P5" s="6"/>
       <c r="Q5" s="4">
-        <f>C5+D5+E5+F5+G5+H5+I5+J5+K5+L5+M5+N5+O5+P5</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="R5" s="7"/>
       <c r="S5" s="8"/>
@@ -1025,14 +1034,17 @@
         <v>70</v>
       </c>
       <c r="C6" s="5"/>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
       <c r="H6" t="b">
         <v>1</v>
       </c>
       <c r="J6" s="18"/>
       <c r="P6" s="6"/>
       <c r="Q6" s="4">
-        <f>C6+D6+E6+F6+G6+H6+I6+J6+K6+L6+M6+N6+O6+P6</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="R6" s="7"/>
       <c r="S6" s="8"/>
@@ -1047,7 +1059,7 @@
       <c r="J7" s="18"/>
       <c r="P7" s="6"/>
       <c r="Q7" s="4">
-        <f>C7+D7+E7+F7+G7+H7+I7+J7+K7+L7+M7+N7+O7+P7</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R7" s="7"/>
@@ -1061,11 +1073,14 @@
       <c r="E8" t="b">
         <v>1</v>
       </c>
+      <c r="H8" t="b">
+        <v>1</v>
+      </c>
       <c r="J8" s="18"/>
       <c r="P8" s="6"/>
       <c r="Q8" s="4">
-        <f>C8+D8+E8+F8+G8+H8+I8+J8+K8+L8+M8+N8+O8+P8</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="R8" s="7"/>
       <c r="S8" s="8"/>
@@ -1081,7 +1096,7 @@
       <c r="J9" s="18"/>
       <c r="P9" s="6"/>
       <c r="Q9" s="4">
-        <f>C9+D9+E9+F9+G9+H9+I9+J9+K9+L9+M9+N9+O9+P9</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R9" s="7"/>
@@ -1101,7 +1116,7 @@
       <c r="J10" s="18"/>
       <c r="P10" s="6"/>
       <c r="Q10" s="4">
-        <f>C10+D10+E10+F10+G10+H10+I10+J10+K10+L10+M10+N10+O10+P10</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R10" s="7"/>
@@ -1121,7 +1136,7 @@
       <c r="J11" s="18"/>
       <c r="P11" s="6"/>
       <c r="Q11" s="4">
-        <f>C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11+P11</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R11" s="7"/>
@@ -1152,7 +1167,7 @@
       <c r="O12" s="18"/>
       <c r="P12" s="21"/>
       <c r="Q12" s="4">
-        <f>C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12+P12</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R12" s="23"/>
@@ -1178,7 +1193,7 @@
       <c r="J13" s="18"/>
       <c r="P13" s="6"/>
       <c r="Q13" s="4">
-        <f>C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13+P13</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="R13" s="7"/>
@@ -1198,7 +1213,7 @@
       <c r="J14" s="18"/>
       <c r="P14" s="6"/>
       <c r="Q14" s="4">
-        <f>C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14+P14</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R14" s="7"/>
@@ -1215,11 +1230,14 @@
       <c r="G15" t="b">
         <v>1</v>
       </c>
+      <c r="H15" t="b">
+        <v>1</v>
+      </c>
       <c r="J15" s="18"/>
       <c r="P15" s="6"/>
       <c r="Q15" s="4">
-        <f>C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15+P15</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="R15" s="9"/>
       <c r="S15" s="10"/>
@@ -1241,7 +1259,7 @@
       <c r="J16" s="18"/>
       <c r="P16" s="6"/>
       <c r="Q16" s="4">
-        <f>C16+D16+E16+F16+G16+H16+I16+J16+K16+L16+M16+N16+O16+P16</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R16" s="7"/>
@@ -1261,11 +1279,14 @@
       <c r="G17" t="b">
         <v>1</v>
       </c>
+      <c r="H17" t="b">
+        <v>1</v>
+      </c>
       <c r="J17" s="18"/>
       <c r="P17" s="6"/>
       <c r="Q17" s="4">
-        <f>C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17+P17</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="R17" s="7"/>
       <c r="S17" s="8"/>
@@ -1280,7 +1301,7 @@
       <c r="J18" s="18"/>
       <c r="P18" s="6"/>
       <c r="Q18" s="4">
-        <f>C18+D18+E18+F18+G18+H18+I18+J18+K18+L18+M18+N18+O18+P18</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R18" s="7"/>
@@ -1311,7 +1332,7 @@
       <c r="J19" s="18"/>
       <c r="P19" s="6"/>
       <c r="Q19" s="4">
-        <f>C19+D19+E19+F19+G19+H19+I19+J19+K19+L19+M19+N19+O19+P19</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="R19" s="7"/>
@@ -1334,7 +1355,7 @@
       <c r="J20" s="18"/>
       <c r="P20" s="6"/>
       <c r="Q20" s="4">
-        <f>C20+D20+E20+F20+G20+H20+I20+J20+K20+L20+M20+N20+O20+P20</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R20" s="7"/>
@@ -1348,11 +1369,14 @@
       <c r="G21" t="b">
         <v>1</v>
       </c>
+      <c r="H21" t="b">
+        <v>1</v>
+      </c>
       <c r="J21" s="18"/>
       <c r="P21" s="6"/>
       <c r="Q21" s="4">
-        <f>C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21+P21</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="R21" s="9"/>
       <c r="S21" s="8"/>
@@ -1374,7 +1398,7 @@
       <c r="J22" s="18"/>
       <c r="P22" s="6"/>
       <c r="Q22" s="4">
-        <f>C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22+P22</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R22" s="7"/>
@@ -1407,7 +1431,7 @@
       <c r="O23" s="18"/>
       <c r="P23" s="21"/>
       <c r="Q23" s="4">
-        <f>C23+D23+E23+F23+G23+H23+I23+J23+K23+L23+M23+N23+O23+P23</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="R23" s="23"/>
@@ -1427,7 +1451,7 @@
       <c r="J24" s="18"/>
       <c r="P24" s="6"/>
       <c r="Q24" s="4">
-        <f>C24+D24+E24+F24+G24+H24+I24+J24+K24+L24+M24+N24+O24+P24</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R24" s="7"/>
@@ -1444,7 +1468,7 @@
       <c r="J25" s="18"/>
       <c r="P25" s="6"/>
       <c r="Q25" s="4">
-        <f>C25+D25+E25+F25+G25+H25+I25+J25+K25+L25+M25+N25+O25+P25</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R25" s="7"/>
@@ -1477,7 +1501,7 @@
       <c r="O26" s="18"/>
       <c r="P26" s="21"/>
       <c r="Q26" s="4">
-        <f>C26+D26+E26+F26+G26+H26+I26+J26+K26+L26+M26+N26+O26+P26</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="R26" s="23"/>
@@ -1497,7 +1521,7 @@
       <c r="J27" s="18"/>
       <c r="P27" s="6"/>
       <c r="Q27" s="4">
-        <f>C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27+P27</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R27" s="7"/>
@@ -1520,7 +1544,7 @@
       <c r="J28" s="18"/>
       <c r="P28" s="6"/>
       <c r="Q28" s="4">
-        <f>C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28+P28</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R28" s="7"/>
@@ -1537,11 +1561,14 @@
       <c r="E29" t="b">
         <v>1</v>
       </c>
+      <c r="H29" t="b">
+        <v>1</v>
+      </c>
       <c r="J29" s="18"/>
       <c r="P29" s="6"/>
       <c r="Q29" s="4">
-        <f>C29+D29+E29+F29+G29+H29+I29+J29+K29+L29+M29+N29+O29+P29</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="R29" s="9"/>
       <c r="S29" s="10"/>
@@ -1563,7 +1590,7 @@
       <c r="J30" s="18"/>
       <c r="P30" s="6"/>
       <c r="Q30" s="4">
-        <f>C30+D30+E30+F30+G30+H30+I30+J30+K30+L30+M30+N30+O30+P30</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R30" s="7"/>
@@ -1580,7 +1607,7 @@
       <c r="J31" s="18"/>
       <c r="P31" s="6"/>
       <c r="Q31" s="4">
-        <f>C31+D31+E31+F31+G31+H31+I31+J31+K31+L31+M31+N31+O31+P31</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R31" s="7"/>
@@ -1600,11 +1627,14 @@
       <c r="G32" t="b">
         <v>1</v>
       </c>
+      <c r="H32" t="b">
+        <v>1</v>
+      </c>
       <c r="J32" s="18"/>
       <c r="P32" s="6"/>
       <c r="Q32" s="4">
-        <f>C32+D32+E32+F32+G32+H32+I32+J32+K32+L32+M32+N32+O32+P32</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="R32" s="7"/>
       <c r="S32" s="8"/>
@@ -1629,7 +1659,7 @@
       <c r="J33" s="18"/>
       <c r="P33" s="6"/>
       <c r="Q33" s="4">
-        <f>C33+D33+E33+F33+G33+H33+I33+J33+K33+L33+M33+N33+O33+P33</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="R33" s="7"/>
@@ -1640,14 +1670,17 @@
         <v>69</v>
       </c>
       <c r="C34" s="5"/>
+      <c r="G34" t="b">
+        <v>1</v>
+      </c>
       <c r="H34" t="b">
         <v>1</v>
       </c>
       <c r="J34" s="18"/>
       <c r="P34" s="6"/>
       <c r="Q34" s="4">
-        <f>C34+D34+E34+F34+G34+H34+I34+J34+K34+L34+M34+N34+O34+P34</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="R34" s="7"/>
       <c r="S34" s="8"/>
@@ -1663,7 +1696,7 @@
       <c r="J35" s="18"/>
       <c r="P35" s="6"/>
       <c r="Q35" s="4">
-        <f>C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
+        <f t="shared" ref="Q35:Q66" si="1">C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
         <v>1</v>
       </c>
       <c r="R35" s="7"/>
@@ -1683,11 +1716,14 @@
       <c r="G36" t="b">
         <v>1</v>
       </c>
+      <c r="H36" t="b">
+        <v>1</v>
+      </c>
       <c r="J36" s="18"/>
       <c r="P36" s="6"/>
       <c r="Q36" s="4">
-        <f>C36+D36+E36+F36+G36+H36+I36+J36+K36+L36+M36+N36+O36+P36</f>
-        <v>3</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="R36" s="7"/>
       <c r="S36" s="8"/>
@@ -1700,11 +1736,14 @@
       <c r="G37" t="b">
         <v>1</v>
       </c>
+      <c r="H37" t="b">
+        <v>1</v>
+      </c>
       <c r="J37" s="18"/>
       <c r="P37" s="6"/>
       <c r="Q37" s="4">
-        <f>C37+D37+E37+F37+G37+H37+I37+J37+K37+L37+M37+N37+O37+P37</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="R37" s="7"/>
       <c r="S37" s="8"/>
@@ -1720,7 +1759,7 @@
       <c r="J38" s="18"/>
       <c r="P38" s="6"/>
       <c r="Q38" s="4">
-        <f>C38+D38+E38+F38+G38+H38+I38+J38+K38+L38+M38+N38+O38+P38</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="R38" s="7"/>
@@ -1740,7 +1779,7 @@
       <c r="J39" s="18"/>
       <c r="P39" s="6"/>
       <c r="Q39" s="4">
-        <f>C39+D39+E39+F39+G39+H39+I39+J39+K39+L39+M39+N39+O39+P39</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="R39" s="9"/>
@@ -1754,6 +1793,9 @@
       <c r="E40" t="b">
         <v>1</v>
       </c>
+      <c r="F40" t="b">
+        <v>1</v>
+      </c>
       <c r="G40" t="b">
         <v>1</v>
       </c>
@@ -1763,8 +1805,8 @@
       <c r="J40" s="18"/>
       <c r="P40" s="6"/>
       <c r="Q40" s="4">
-        <f>C40+D40+E40+F40+G40+H40+I40+J40+K40+L40+M40+N40+O40+P40</f>
-        <v>3</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="R40" s="7"/>
       <c r="S40" s="8"/>
@@ -1783,7 +1825,7 @@
       <c r="J41" s="18"/>
       <c r="P41" s="6"/>
       <c r="Q41" s="4">
-        <f>C41+D41+E41+F41+G41+H41+I41+J41+K41+L41+M41+N41+O41+P41</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="R41" s="7"/>
@@ -1803,11 +1845,14 @@
       <c r="G42" t="b">
         <v>1</v>
       </c>
+      <c r="H42" t="b">
+        <v>1</v>
+      </c>
       <c r="J42" s="18"/>
       <c r="P42" s="6"/>
       <c r="Q42" s="4">
-        <f>C42+D42+E42+F42+G42+H42+I42+J42+K42+L42+M42+N42+O42+P42</f>
-        <v>3</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="R42" s="7"/>
       <c r="S42" s="8"/>
@@ -1828,11 +1873,14 @@
       <c r="G43" t="b">
         <v>1</v>
       </c>
+      <c r="H43" t="b">
+        <v>1</v>
+      </c>
       <c r="J43" s="18"/>
       <c r="P43" s="6"/>
       <c r="Q43" s="4">
-        <f>C43+D43+E43+F43+G43+H43+I43+J43+K43+L43+M43+N43+O43+P43</f>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
       <c r="R43" s="7"/>
       <c r="S43" s="8"/>
@@ -1854,7 +1902,7 @@
       <c r="J44" s="18"/>
       <c r="P44" s="6"/>
       <c r="Q44" s="4">
-        <f>C44+D44+E44+F44+G44+H44+I44+J44+K44+L44+M44+N44+O44+P44</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="R44" s="7"/>
@@ -1874,7 +1922,7 @@
       <c r="J45" s="18"/>
       <c r="P45" s="6"/>
       <c r="Q45" s="4">
-        <f>C45+D45+E45+F45+G45+H45+I45+J45+K45+L45+M45+N45+O45+P45</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="R45" s="7"/>
@@ -1893,11 +1941,14 @@
       <c r="G46" t="b">
         <v>1</v>
       </c>
+      <c r="H46" t="b">
+        <v>1</v>
+      </c>
       <c r="J46" s="18"/>
       <c r="P46" s="6"/>
       <c r="Q46" s="4">
-        <f>C46+D46+E46+F46+G46+H46+I46+J46+K46+L46+M46+N46+O46+P46</f>
-        <v>3</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="R46" s="9"/>
       <c r="S46" s="10"/>
@@ -1922,7 +1973,7 @@
       <c r="J47" s="18"/>
       <c r="P47" s="6"/>
       <c r="Q47" s="4">
-        <f>C47+D47+E47+F47+G47+H47+I47+J47+K47+L47+M47+N47+O47+P47</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="R47" s="7"/>
@@ -1945,11 +1996,14 @@
       <c r="G48" t="b">
         <v>1</v>
       </c>
+      <c r="H48" t="b">
+        <v>1</v>
+      </c>
       <c r="J48" s="18"/>
       <c r="P48" s="6"/>
       <c r="Q48" s="4">
-        <f>C48+D48+E48+F48+G48+H48+I48+J48+K48+L48+M48+N48+O48+P48</f>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
       <c r="R48" s="7"/>
       <c r="S48" s="8"/>
@@ -1971,11 +2025,14 @@
       <c r="G49" t="b">
         <v>1</v>
       </c>
+      <c r="H49" t="b">
+        <v>1</v>
+      </c>
       <c r="J49" s="18"/>
       <c r="P49" s="6"/>
       <c r="Q49" s="4">
-        <f>C49+D49+E49+F49+G49+H49+I49+J49+K49+L49+M49+N49+O49+P49</f>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
       <c r="R49" s="7"/>
       <c r="S49" s="8"/>
@@ -1994,7 +2051,7 @@
       <c r="J50" s="18"/>
       <c r="P50" s="6"/>
       <c r="Q50" s="4">
-        <f>C50+D50+E50+F50+G50+H50+I50+J50+K50+L50+M50+N50+O50+P50</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="R50" s="7"/>
@@ -2008,11 +2065,14 @@
       <c r="G51" t="b">
         <v>1</v>
       </c>
+      <c r="H51" t="b">
+        <v>1</v>
+      </c>
       <c r="J51" s="18"/>
       <c r="P51" s="6"/>
       <c r="Q51" s="4">
-        <f>C51+D51+E51+F51+G51+H51+I51+J51+K51+L51+M51+N51+O51+P51</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="R51" s="7"/>
       <c r="S51" s="8"/>
@@ -2037,7 +2097,7 @@
       <c r="J52" s="18"/>
       <c r="P52" s="6"/>
       <c r="Q52" s="4">
-        <f>C52+D52+E52+F52+G52+H52+I52+J52+K52+L52+M52+N52+O52+P52</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="R52" s="7"/>
@@ -2057,7 +2117,7 @@
       <c r="J53" s="18"/>
       <c r="P53" s="6"/>
       <c r="Q53" s="4">
-        <f>C53+D53+E53+F53+G53+H53+I53+J53+K53+L53+M53+N53+O53+P53</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="R53" s="7"/>
@@ -2088,7 +2148,7 @@
       <c r="O54" s="18"/>
       <c r="P54" s="21"/>
       <c r="Q54" s="4">
-        <f>C54+D54+E54+F54+G54+H54+I54+J54+K54+L54+M54+N54+O54+P54</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="R54" s="25"/>
@@ -2110,23 +2170,31 @@
       <c r="F55" t="b">
         <v>1</v>
       </c>
+      <c r="H55" t="b">
+        <v>1</v>
+      </c>
       <c r="J55" s="18"/>
       <c r="P55" s="6"/>
       <c r="Q55" s="4">
-        <f>C55+D55+E55+F55+G55+H55+I55+J55+K55+L55+M55+N55+O55+P55</f>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
       <c r="R55" s="7"/>
       <c r="S55" s="8"/>
     </row>
     <row r="56" spans="2:19">
-      <c r="B56" s="3"/>
+      <c r="B56" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="C56" s="5"/>
+      <c r="H56" t="b">
+        <v>1</v>
+      </c>
       <c r="J56" s="18"/>
       <c r="P56" s="6"/>
       <c r="Q56" s="4">
-        <f t="shared" ref="Q52:Q57" si="0">C56+D56+E56+F56+G56+H56+I56+J56+K56+L56+M56+N56+O56+P56</f>
-        <v>0</v>
+        <f t="shared" ref="Q56:Q57" si="2">C56+D56+E56+F56+G56+H56+I56+J56+K56+L56+M56+N56+O56+P56</f>
+        <v>1</v>
       </c>
       <c r="R56" s="7"/>
       <c r="S56" s="8"/>
@@ -2148,7 +2216,7 @@
       <c r="O57" s="12"/>
       <c r="P57" s="13"/>
       <c r="Q57" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R57" s="14"/>

</xml_diff>

<commit_message>
euler + hamilton; edit si create in acelasi formular, mai multe pagini, navigare intre ele
</commit_message>
<xml_diff>
--- a/MetodeAvansateDeProgramare/Prezenta_AnII_2024.xlsx
+++ b/MetodeAvansateDeProgramare/Prezenta_AnII_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_Promotia_2023_2026\MetodeAvansateDeProgramare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61FBD99D-4414-49CC-B3B2-DC847BA5B190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339E87B2-E655-43F5-B359-FDD34D8CD1DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>Proiect</t>
   </si>
@@ -241,6 +241,9 @@
   </si>
   <si>
     <t>Victor Balaj</t>
+  </si>
+  <si>
+    <t>Alexandra Iovan</t>
   </si>
 </sst>
 </file>
@@ -875,7 +878,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M15" sqref="M15"/>
+      <selection pane="bottomRight" activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -994,11 +997,16 @@
       <c r="H4" t="b">
         <v>1</v>
       </c>
-      <c r="J4" s="18"/>
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" s="18" t="b">
+        <v>1</v>
+      </c>
       <c r="P4" s="6"/>
       <c r="Q4" s="4">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="R4" s="9"/>
       <c r="S4" s="10"/>
@@ -1020,11 +1028,14 @@
       <c r="H5" t="b">
         <v>1</v>
       </c>
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
       <c r="J5" s="18"/>
       <c r="P5" s="6"/>
       <c r="Q5" s="4">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R5" s="7"/>
       <c r="S5" s="8"/>
@@ -1056,11 +1067,14 @@
       <c r="C7" s="5" t="b">
         <v>1</v>
       </c>
+      <c r="I7" t="b">
+        <v>1</v>
+      </c>
       <c r="J7" s="18"/>
       <c r="P7" s="6"/>
       <c r="Q7" s="4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R7" s="7"/>
       <c r="S7" s="8"/>
@@ -1073,14 +1087,20 @@
       <c r="E8" t="b">
         <v>1</v>
       </c>
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
       <c r="H8" t="b">
+        <v>1</v>
+      </c>
+      <c r="I8" t="b">
         <v>1</v>
       </c>
       <c r="J8" s="18"/>
       <c r="P8" s="6"/>
       <c r="Q8" s="4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R8" s="7"/>
       <c r="S8" s="8"/>
@@ -1093,11 +1113,14 @@
       <c r="D9" t="b">
         <v>1</v>
       </c>
+      <c r="I9" t="b">
+        <v>1</v>
+      </c>
       <c r="J9" s="18"/>
       <c r="P9" s="6"/>
       <c r="Q9" s="4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R9" s="7"/>
       <c r="S9" s="8"/>
@@ -1133,11 +1156,14 @@
       <c r="H11" t="b">
         <v>1</v>
       </c>
+      <c r="I11" t="b">
+        <v>1</v>
+      </c>
       <c r="J11" s="18"/>
       <c r="P11" s="6"/>
       <c r="Q11" s="4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R11" s="7"/>
       <c r="S11" s="8"/>
@@ -1158,7 +1184,9 @@
       <c r="H12" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="I12" s="18"/>
+      <c r="I12" s="18" t="b">
+        <v>1</v>
+      </c>
       <c r="J12" s="18"/>
       <c r="K12" s="18"/>
       <c r="L12" s="18"/>
@@ -1168,7 +1196,7 @@
       <c r="P12" s="21"/>
       <c r="Q12" s="4">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R12" s="23"/>
       <c r="S12" s="24"/>
@@ -1190,11 +1218,14 @@
       <c r="H13" t="b">
         <v>1</v>
       </c>
+      <c r="I13" t="b">
+        <v>1</v>
+      </c>
       <c r="J13" s="18"/>
       <c r="P13" s="6"/>
       <c r="Q13" s="4">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R13" s="7"/>
       <c r="S13" s="8"/>
@@ -1207,14 +1238,20 @@
       <c r="E14" t="b">
         <v>1</v>
       </c>
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
       <c r="H14" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" t="b">
         <v>1</v>
       </c>
       <c r="J14" s="18"/>
       <c r="P14" s="6"/>
       <c r="Q14" s="4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R14" s="7"/>
       <c r="S14" s="8"/>
@@ -1227,17 +1264,23 @@
       <c r="E15" t="b">
         <v>1</v>
       </c>
+      <c r="F15" t="b">
+        <v>1</v>
+      </c>
       <c r="G15" t="b">
         <v>1</v>
       </c>
       <c r="H15" t="b">
+        <v>1</v>
+      </c>
+      <c r="I15" t="b">
         <v>1</v>
       </c>
       <c r="J15" s="18"/>
       <c r="P15" s="6"/>
       <c r="Q15" s="4">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="R15" s="9"/>
       <c r="S15" s="10"/>
@@ -1256,11 +1299,14 @@
       <c r="H16" t="b">
         <v>1</v>
       </c>
+      <c r="I16" t="b">
+        <v>1</v>
+      </c>
       <c r="J16" s="18"/>
       <c r="P16" s="6"/>
       <c r="Q16" s="4">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R16" s="7"/>
       <c r="S16" s="8"/>
@@ -1270,6 +1316,9 @@
         <v>54</v>
       </c>
       <c r="C17" s="5"/>
+      <c r="D17" t="b">
+        <v>1</v>
+      </c>
       <c r="E17" t="b">
         <v>1</v>
       </c>
@@ -1280,13 +1329,16 @@
         <v>1</v>
       </c>
       <c r="H17" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17" t="b">
         <v>1</v>
       </c>
       <c r="J17" s="18"/>
       <c r="P17" s="6"/>
       <c r="Q17" s="4">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="R17" s="7"/>
       <c r="S17" s="8"/>
@@ -1329,11 +1381,14 @@
       <c r="H19" t="b">
         <v>1</v>
       </c>
+      <c r="I19" t="b">
+        <v>1</v>
+      </c>
       <c r="J19" s="18"/>
       <c r="P19" s="6"/>
       <c r="Q19" s="4">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R19" s="7"/>
       <c r="S19" s="8"/>
@@ -1352,11 +1407,14 @@
       <c r="G20" t="b">
         <v>1</v>
       </c>
+      <c r="I20" t="b">
+        <v>1</v>
+      </c>
       <c r="J20" s="18"/>
       <c r="P20" s="6"/>
       <c r="Q20" s="4">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R20" s="7"/>
       <c r="S20" s="8"/>
@@ -1372,11 +1430,14 @@
       <c r="H21" t="b">
         <v>1</v>
       </c>
+      <c r="I21" t="b">
+        <v>1</v>
+      </c>
       <c r="J21" s="18"/>
       <c r="P21" s="6"/>
       <c r="Q21" s="4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R21" s="9"/>
       <c r="S21" s="8"/>
@@ -1395,11 +1456,14 @@
       <c r="G22" t="b">
         <v>1</v>
       </c>
+      <c r="I22" t="b">
+        <v>1</v>
+      </c>
       <c r="J22" s="18"/>
       <c r="P22" s="6"/>
       <c r="Q22" s="4">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R22" s="7"/>
       <c r="S22" s="8"/>
@@ -1422,7 +1486,9 @@
         <v>1</v>
       </c>
       <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
+      <c r="I23" s="18" t="b">
+        <v>1</v>
+      </c>
       <c r="J23" s="18"/>
       <c r="K23" s="18"/>
       <c r="L23" s="18"/>
@@ -1432,7 +1498,7 @@
       <c r="P23" s="21"/>
       <c r="Q23" s="4">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R23" s="23"/>
       <c r="S23" s="31"/>
@@ -1445,14 +1511,20 @@
       <c r="E24" t="b">
         <v>1</v>
       </c>
+      <c r="G24" t="b">
+        <v>1</v>
+      </c>
       <c r="H24" t="b">
+        <v>1</v>
+      </c>
+      <c r="I24" t="b">
         <v>1</v>
       </c>
       <c r="J24" s="18"/>
       <c r="P24" s="6"/>
       <c r="Q24" s="4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R24" s="7"/>
       <c r="S24" s="8"/>
@@ -1492,7 +1564,9 @@
       </c>
       <c r="G26" s="18"/>
       <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
+      <c r="I26" s="18" t="b">
+        <v>1</v>
+      </c>
       <c r="J26" s="18"/>
       <c r="K26" s="18"/>
       <c r="L26" s="18"/>
@@ -1502,7 +1576,7 @@
       <c r="P26" s="21"/>
       <c r="Q26" s="4">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R26" s="23"/>
       <c r="S26" s="31"/>
@@ -1564,11 +1638,14 @@
       <c r="H29" t="b">
         <v>1</v>
       </c>
+      <c r="I29" t="b">
+        <v>1</v>
+      </c>
       <c r="J29" s="18"/>
       <c r="P29" s="6"/>
       <c r="Q29" s="4">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R29" s="9"/>
       <c r="S29" s="10"/>
@@ -1587,11 +1664,14 @@
       <c r="G30" t="b">
         <v>1</v>
       </c>
+      <c r="I30" t="b">
+        <v>1</v>
+      </c>
       <c r="J30" s="18"/>
       <c r="P30" s="6"/>
       <c r="Q30" s="4">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R30" s="7"/>
       <c r="S30" s="8"/>
@@ -1630,11 +1710,14 @@
       <c r="H32" t="b">
         <v>1</v>
       </c>
+      <c r="I32" t="b">
+        <v>1</v>
+      </c>
       <c r="J32" s="18"/>
       <c r="P32" s="6"/>
       <c r="Q32" s="4">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R32" s="7"/>
       <c r="S32" s="8"/>
@@ -1656,11 +1739,14 @@
       <c r="H33" t="b">
         <v>1</v>
       </c>
+      <c r="I33" t="b">
+        <v>1</v>
+      </c>
       <c r="J33" s="18"/>
       <c r="P33" s="6"/>
       <c r="Q33" s="4">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R33" s="7"/>
       <c r="S33" s="8"/>
@@ -1670,17 +1756,23 @@
         <v>69</v>
       </c>
       <c r="C34" s="5"/>
+      <c r="F34" t="b">
+        <v>1</v>
+      </c>
       <c r="G34" t="b">
         <v>1</v>
       </c>
       <c r="H34" t="b">
+        <v>1</v>
+      </c>
+      <c r="I34" t="b">
         <v>1</v>
       </c>
       <c r="J34" s="18"/>
       <c r="P34" s="6"/>
       <c r="Q34" s="4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R34" s="7"/>
       <c r="S34" s="8"/>
@@ -1693,11 +1785,14 @@
       <c r="H35" t="b">
         <v>1</v>
       </c>
+      <c r="I35" t="b">
+        <v>1</v>
+      </c>
       <c r="J35" s="18"/>
       <c r="P35" s="6"/>
       <c r="Q35" s="4">
-        <f t="shared" ref="Q35:Q66" si="1">C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
-        <v>1</v>
+        <f t="shared" ref="Q35:Q55" si="1">C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
+        <v>2</v>
       </c>
       <c r="R35" s="7"/>
       <c r="S35" s="8"/>
@@ -1707,6 +1802,9 @@
         <v>44</v>
       </c>
       <c r="C36" s="5"/>
+      <c r="D36" t="b">
+        <v>1</v>
+      </c>
       <c r="E36" t="b">
         <v>1</v>
       </c>
@@ -1717,13 +1815,16 @@
         <v>1</v>
       </c>
       <c r="H36" t="b">
+        <v>1</v>
+      </c>
+      <c r="I36" t="b">
         <v>1</v>
       </c>
       <c r="J36" s="18"/>
       <c r="P36" s="6"/>
       <c r="Q36" s="4">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="R36" s="7"/>
       <c r="S36" s="8"/>
@@ -1737,13 +1838,16 @@
         <v>1</v>
       </c>
       <c r="H37" t="b">
+        <v>1</v>
+      </c>
+      <c r="I37" t="b">
         <v>1</v>
       </c>
       <c r="J37" s="18"/>
       <c r="P37" s="6"/>
       <c r="Q37" s="4">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R37" s="7"/>
       <c r="S37" s="8"/>
@@ -1790,6 +1894,9 @@
         <v>47</v>
       </c>
       <c r="C40" s="5"/>
+      <c r="D40" t="b">
+        <v>1</v>
+      </c>
       <c r="E40" t="b">
         <v>1</v>
       </c>
@@ -1800,13 +1907,16 @@
         <v>1</v>
       </c>
       <c r="H40" t="b">
+        <v>1</v>
+      </c>
+      <c r="I40" t="b">
         <v>1</v>
       </c>
       <c r="J40" s="18"/>
       <c r="P40" s="6"/>
       <c r="Q40" s="4">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="R40" s="7"/>
       <c r="S40" s="8"/>
@@ -1848,11 +1958,14 @@
       <c r="H42" t="b">
         <v>1</v>
       </c>
+      <c r="I42" t="b">
+        <v>1</v>
+      </c>
       <c r="J42" s="18"/>
       <c r="P42" s="6"/>
       <c r="Q42" s="4">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R42" s="7"/>
       <c r="S42" s="8"/>
@@ -1874,13 +1987,16 @@
         <v>1</v>
       </c>
       <c r="H43" t="b">
+        <v>1</v>
+      </c>
+      <c r="I43" t="b">
         <v>1</v>
       </c>
       <c r="J43" s="18"/>
       <c r="P43" s="6"/>
       <c r="Q43" s="4">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R43" s="7"/>
       <c r="S43" s="8"/>
@@ -1919,11 +2035,14 @@
       <c r="H45" t="b">
         <v>1</v>
       </c>
+      <c r="I45" t="b">
+        <v>1</v>
+      </c>
       <c r="J45" s="18"/>
       <c r="P45" s="6"/>
       <c r="Q45" s="4">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R45" s="7"/>
       <c r="S45" s="8"/>
@@ -1970,11 +2089,14 @@
       <c r="H47" t="b">
         <v>1</v>
       </c>
+      <c r="I47" t="b">
+        <v>1</v>
+      </c>
       <c r="J47" s="18"/>
       <c r="P47" s="6"/>
       <c r="Q47" s="4">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R47" s="7"/>
       <c r="S47" s="8"/>
@@ -1997,13 +2119,16 @@
         <v>1</v>
       </c>
       <c r="H48" t="b">
+        <v>1</v>
+      </c>
+      <c r="I48" t="b">
         <v>1</v>
       </c>
       <c r="J48" s="18"/>
       <c r="P48" s="6"/>
       <c r="Q48" s="4">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R48" s="7"/>
       <c r="S48" s="8"/>
@@ -2068,11 +2193,14 @@
       <c r="H51" t="b">
         <v>1</v>
       </c>
+      <c r="I51" t="b">
+        <v>1</v>
+      </c>
       <c r="J51" s="18"/>
       <c r="P51" s="6"/>
       <c r="Q51" s="4">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R51" s="7"/>
       <c r="S51" s="8"/>
@@ -2092,13 +2220,16 @@
         <v>1</v>
       </c>
       <c r="H52" t="b">
+        <v>1</v>
+      </c>
+      <c r="I52" t="b">
         <v>1</v>
       </c>
       <c r="J52" s="18"/>
       <c r="P52" s="6"/>
       <c r="Q52" s="4">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R52" s="7"/>
       <c r="S52" s="8"/>
@@ -2112,13 +2243,16 @@
         <v>1</v>
       </c>
       <c r="H53" t="b">
+        <v>1</v>
+      </c>
+      <c r="I53" t="b">
         <v>1</v>
       </c>
       <c r="J53" s="18"/>
       <c r="P53" s="6"/>
       <c r="Q53" s="4">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R53" s="7"/>
       <c r="S53" s="8"/>
@@ -2139,7 +2273,9 @@
       <c r="H54" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="I54" s="18"/>
+      <c r="I54" s="18" t="b">
+        <v>1</v>
+      </c>
       <c r="J54" s="18"/>
       <c r="K54" s="18"/>
       <c r="L54" s="18"/>
@@ -2149,7 +2285,7 @@
       <c r="P54" s="21"/>
       <c r="Q54" s="4">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R54" s="25"/>
       <c r="S54" s="24"/>
@@ -2200,14 +2336,18 @@
       <c r="S56" s="8"/>
     </row>
     <row r="57" spans="2:19">
-      <c r="B57" s="29"/>
+      <c r="B57" s="29" t="s">
+        <v>72</v>
+      </c>
       <c r="C57" s="11"/>
       <c r="D57" s="12"/>
       <c r="E57" s="12"/>
       <c r="F57" s="12"/>
       <c r="G57" s="12"/>
       <c r="H57" s="12"/>
-      <c r="I57" s="12"/>
+      <c r="I57" s="12" t="b">
+        <v>1</v>
+      </c>
       <c r="J57" s="22"/>
       <c r="K57" s="12"/>
       <c r="L57" s="12"/>
@@ -2217,7 +2357,7 @@
       <c r="P57" s="13"/>
       <c r="Q57" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R57" s="14"/>
       <c r="S57" s="15"/>

</xml_diff>

<commit_message>
am adaugat services pentru managementul datelor, si am inceput sa lucram la cum arata PDF-ul
</commit_message>
<xml_diff>
--- a/MetodeAvansateDeProgramare/Prezenta_AnII_2024.xlsx
+++ b/MetodeAvansateDeProgramare/Prezenta_AnII_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_Promotia_2023_2026\MetodeAvansateDeProgramare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{091A136A-DB39-4403-8137-36D4F5AE1674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F98AB062-0D21-4D5A-8856-C85C7AF216C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -502,7 +502,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -581,7 +581,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -876,11 +875,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:S58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C42" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H50" sqref="H50"/>
+      <selection pane="bottomRight" activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -971,7 +970,7 @@
       <c r="O3" s="17"/>
       <c r="P3" s="31"/>
       <c r="Q3" s="4">
-        <f>C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
+        <f t="shared" ref="Q3:Q34" si="0">C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
         <v>2</v>
       </c>
       <c r="R3" s="32"/>
@@ -982,25 +981,15 @@
         <v>72</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34" t="b">
+      <c r="I4" t="b">
         <v>1</v>
       </c>
       <c r="J4" s="16" t="b">
         <v>1</v>
       </c>
-      <c r="K4" s="34"/>
-      <c r="L4" s="34"/>
-      <c r="M4" s="34"/>
-      <c r="N4" s="34"/>
-      <c r="O4" s="34"/>
       <c r="P4" s="6"/>
       <c r="Q4" s="4">
-        <f>C4+D4+E4+F4+G4+H4+I4+J4+K4+L4+M4+N4+O4+P4</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R4" s="7"/>
@@ -1039,7 +1028,7 @@
       </c>
       <c r="P5" s="6"/>
       <c r="Q5" s="4">
-        <f>C5+D5+E5+F5+G5+H5+I5+J5+K5+L5+M5+N5+O5+P5</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="R5" s="9"/>
@@ -1065,11 +1054,13 @@
       <c r="I6" t="b">
         <v>1</v>
       </c>
-      <c r="J6" s="16"/>
+      <c r="J6" s="16" t="b">
+        <v>1</v>
+      </c>
       <c r="P6" s="6"/>
       <c r="Q6" s="4">
-        <f>C6+D6+E6+F6+G6+H6+I6+J6+K6+L6+M6+N6+O6+P6</f>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="R6" s="7"/>
       <c r="S6" s="8"/>
@@ -1088,7 +1079,7 @@
       <c r="J7" s="16"/>
       <c r="P7" s="6"/>
       <c r="Q7" s="4">
-        <f>C7+D7+E7+F7+G7+H7+I7+J7+K7+L7+M7+N7+O7+P7</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R7" s="7"/>
@@ -1109,7 +1100,7 @@
       </c>
       <c r="P8" s="6"/>
       <c r="Q8" s="4">
-        <f>C8+D8+E8+F8+G8+H8+I8+J8+K8+L8+M8+N8+O8+P8</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R8" s="7"/>
@@ -1123,6 +1114,9 @@
       <c r="E9" t="b">
         <v>1</v>
       </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
       <c r="G9" t="b">
         <v>1</v>
       </c>
@@ -1137,8 +1131,8 @@
       </c>
       <c r="P9" s="6"/>
       <c r="Q9" s="4">
-        <f>C9+D9+E9+F9+G9+H9+I9+J9+K9+L9+M9+N9+O9+P9</f>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="R9" s="7"/>
       <c r="S9" s="8"/>
@@ -1154,11 +1148,13 @@
       <c r="I10" t="b">
         <v>1</v>
       </c>
-      <c r="J10" s="16"/>
+      <c r="J10" s="16" t="b">
+        <v>1</v>
+      </c>
       <c r="P10" s="6"/>
       <c r="Q10" s="4">
-        <f>C10+D10+E10+F10+G10+H10+I10+J10+K10+L10+M10+N10+O10+P10</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="R10" s="7"/>
       <c r="S10" s="8"/>
@@ -1177,7 +1173,7 @@
       <c r="J11" s="16"/>
       <c r="P11" s="6"/>
       <c r="Q11" s="4">
-        <f>C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11+P11</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R11" s="7"/>
@@ -1200,7 +1196,7 @@
       <c r="J12" s="16"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="4">
-        <f>C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12+P12</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R12" s="7"/>
@@ -1235,7 +1231,7 @@
       <c r="O13" s="16"/>
       <c r="P13" s="19"/>
       <c r="Q13" s="4">
-        <f>C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13+P13</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="R13" s="21"/>
@@ -1266,7 +1262,7 @@
       </c>
       <c r="P14" s="6"/>
       <c r="Q14" s="4">
-        <f>C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14+P14</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="R14" s="7"/>
@@ -1294,7 +1290,7 @@
       </c>
       <c r="P15" s="6"/>
       <c r="Q15" s="4">
-        <f>C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15+P15</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="R15" s="7"/>
@@ -1305,6 +1301,9 @@
         <v>46</v>
       </c>
       <c r="C16" s="5"/>
+      <c r="D16" t="b">
+        <v>1</v>
+      </c>
       <c r="E16" t="b">
         <v>1</v>
       </c>
@@ -1325,8 +1324,8 @@
       </c>
       <c r="P16" s="6"/>
       <c r="Q16" s="4">
-        <f>C16+D16+E16+F16+G16+H16+I16+J16+K16+L16+M16+N16+O16+P16</f>
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="R16" s="9"/>
       <c r="S16" s="10"/>
@@ -1348,11 +1347,13 @@
       <c r="I17" t="b">
         <v>1</v>
       </c>
-      <c r="J17" s="16"/>
+      <c r="J17" s="16" t="b">
+        <v>1</v>
+      </c>
       <c r="P17" s="6"/>
       <c r="Q17" s="4">
-        <f>C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17+P17</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="R17" s="7"/>
       <c r="S17" s="8"/>
@@ -1380,11 +1381,13 @@
       <c r="I18" t="b">
         <v>1</v>
       </c>
-      <c r="J18" s="16"/>
+      <c r="J18" s="16" t="b">
+        <v>1</v>
+      </c>
       <c r="P18" s="6"/>
       <c r="Q18" s="4">
-        <f>C18+D18+E18+F18+G18+H18+I18+J18+K18+L18+M18+N18+O18+P18</f>
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="R18" s="7"/>
       <c r="S18" s="8"/>
@@ -1399,7 +1402,7 @@
       <c r="J19" s="16"/>
       <c r="P19" s="6"/>
       <c r="Q19" s="4">
-        <f>C19+D19+E19+F19+G19+H19+I19+J19+K19+L19+M19+N19+O19+P19</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R19" s="7"/>
@@ -1430,11 +1433,13 @@
       <c r="I20" t="b">
         <v>1</v>
       </c>
-      <c r="J20" s="16"/>
+      <c r="J20" s="16" t="b">
+        <v>1</v>
+      </c>
       <c r="P20" s="6"/>
       <c r="Q20" s="4">
-        <f>C20+D20+E20+F20+G20+H20+I20+J20+K20+L20+M20+N20+O20+P20</f>
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
       <c r="R20" s="7"/>
       <c r="S20" s="8"/>
@@ -1461,7 +1466,7 @@
       </c>
       <c r="P21" s="6"/>
       <c r="Q21" s="4">
-        <f>C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21+P21</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="R21" s="7"/>
@@ -1484,7 +1489,7 @@
       <c r="J22" s="16"/>
       <c r="P22" s="6"/>
       <c r="Q22" s="4">
-        <f>C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22+P22</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="R22" s="9"/>
@@ -1510,7 +1515,7 @@
       <c r="J23" s="16"/>
       <c r="P23" s="6"/>
       <c r="Q23" s="4">
-        <f>C23+D23+E23+F23+G23+H23+I23+J23+K23+L23+M23+N23+O23+P23</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="R23" s="7"/>
@@ -1537,7 +1542,9 @@
       <c r="I24" s="16" t="b">
         <v>1</v>
       </c>
-      <c r="J24" s="16"/>
+      <c r="J24" s="16" t="b">
+        <v>1</v>
+      </c>
       <c r="K24" s="16"/>
       <c r="L24" s="16"/>
       <c r="M24" s="16"/>
@@ -1545,8 +1552,8 @@
       <c r="O24" s="16"/>
       <c r="P24" s="19"/>
       <c r="Q24" s="4">
-        <f>C24+D24+E24+F24+G24+H24+I24+J24+K24+L24+M24+N24+O24+P24</f>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="R24" s="21"/>
       <c r="S24" s="28"/>
@@ -1573,7 +1580,7 @@
       </c>
       <c r="P25" s="6"/>
       <c r="Q25" s="4">
-        <f>C25+D25+E25+F25+G25+H25+I25+J25+K25+L25+M25+N25+O25+P25</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="R25" s="7"/>
@@ -1592,7 +1599,7 @@
       </c>
       <c r="P26" s="6"/>
       <c r="Q26" s="4">
-        <f>C26+D26+E26+F26+G26+H26+I26+J26+K26+L26+M26+N26+O26+P26</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R26" s="7"/>
@@ -1627,7 +1634,7 @@
       <c r="O27" s="16"/>
       <c r="P27" s="19"/>
       <c r="Q27" s="4">
-        <f>C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27+P27</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="R27" s="21"/>
@@ -1638,23 +1645,12 @@
         <v>73</v>
       </c>
       <c r="C28" s="5"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="34"/>
       <c r="J28" s="16" t="b">
         <v>1</v>
       </c>
-      <c r="K28" s="34"/>
-      <c r="L28" s="34"/>
-      <c r="M28" s="34"/>
-      <c r="N28" s="34"/>
-      <c r="O28" s="34"/>
       <c r="P28" s="6"/>
       <c r="Q28" s="4">
-        <f>C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28+P28</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R28" s="9"/>
@@ -1671,13 +1667,16 @@
       <c r="H29" t="b">
         <v>1</v>
       </c>
+      <c r="I29" t="b">
+        <v>1</v>
+      </c>
       <c r="J29" s="16" t="b">
         <v>1</v>
       </c>
       <c r="P29" s="6"/>
       <c r="Q29" s="4">
-        <f>C29+D29+E29+F29+G29+H29+I29+J29+K29+L29+M29+N29+O29+P29</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="R29" s="7"/>
       <c r="S29" s="8"/>
@@ -1701,7 +1700,7 @@
       </c>
       <c r="P30" s="6"/>
       <c r="Q30" s="4">
-        <f>C30+D30+E30+F30+G30+H30+I30+J30+K30+L30+M30+N30+O30+P30</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="R30" s="7"/>
@@ -1724,11 +1723,13 @@
       <c r="I31" t="b">
         <v>1</v>
       </c>
-      <c r="J31" s="16"/>
+      <c r="J31" s="16" t="b">
+        <v>1</v>
+      </c>
       <c r="P31" s="6"/>
       <c r="Q31" s="4">
-        <f>C31+D31+E31+F31+G31+H31+I31+J31+K31+L31+M31+N31+O31+P31</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="R31" s="9"/>
       <c r="S31" s="10"/>
@@ -1753,7 +1754,7 @@
       <c r="J32" s="16"/>
       <c r="P32" s="6"/>
       <c r="Q32" s="4">
-        <f>C32+D32+E32+F32+G32+H32+I32+J32+K32+L32+M32+N32+O32+P32</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="R32" s="7"/>
@@ -1770,7 +1771,7 @@
       <c r="J33" s="16"/>
       <c r="P33" s="6"/>
       <c r="Q33" s="4">
-        <f>C33+D33+E33+F33+G33+H33+I33+J33+K33+L33+M33+N33+O33+P33</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R33" s="7"/>
@@ -1796,11 +1797,13 @@
       <c r="I34" t="b">
         <v>1</v>
       </c>
-      <c r="J34" s="16"/>
+      <c r="J34" s="16" t="b">
+        <v>1</v>
+      </c>
       <c r="P34" s="6"/>
       <c r="Q34" s="4">
-        <f>C34+D34+E34+F34+G34+H34+I34+J34+K34+L34+M34+N34+O34+P34</f>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="R34" s="7"/>
       <c r="S34" s="8"/>
@@ -1830,7 +1833,7 @@
       </c>
       <c r="P35" s="6"/>
       <c r="Q35" s="4">
-        <f>C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
+        <f t="shared" ref="Q35:Q66" si="1">C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
         <v>6</v>
       </c>
       <c r="R35" s="7"/>
@@ -1841,6 +1844,9 @@
         <v>69</v>
       </c>
       <c r="C36" s="5"/>
+      <c r="E36" t="b">
+        <v>1</v>
+      </c>
       <c r="F36" t="b">
         <v>1</v>
       </c>
@@ -1858,8 +1864,8 @@
       </c>
       <c r="P36" s="6"/>
       <c r="Q36" s="4">
-        <f>C36+D36+E36+F36+G36+H36+I36+J36+K36+L36+M36+N36+O36+P36</f>
-        <v>5</v>
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="R36" s="7"/>
       <c r="S36" s="8"/>
@@ -1875,11 +1881,13 @@
       <c r="I37" t="b">
         <v>1</v>
       </c>
-      <c r="J37" s="16"/>
+      <c r="J37" s="16" t="b">
+        <v>1</v>
+      </c>
       <c r="P37" s="6"/>
       <c r="Q37" s="4">
-        <f>C37+D37+E37+F37+G37+H37+I37+J37+K37+L37+M37+N37+O37+P37</f>
-        <v>2</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="R37" s="7"/>
       <c r="S37" s="8"/>
@@ -1912,7 +1920,7 @@
       </c>
       <c r="P38" s="6"/>
       <c r="Q38" s="4">
-        <f>C38+D38+E38+F38+G38+H38+I38+J38+K38+L38+M38+N38+O38+P38</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="R38" s="7"/>
@@ -1932,11 +1940,13 @@
       <c r="I39" t="b">
         <v>1</v>
       </c>
-      <c r="J39" s="16"/>
+      <c r="J39" s="16" t="b">
+        <v>1</v>
+      </c>
       <c r="P39" s="6"/>
       <c r="Q39" s="4">
-        <f>C39+D39+E39+F39+G39+H39+I39+J39+K39+L39+M39+N39+O39+P39</f>
-        <v>3</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="R39" s="7"/>
       <c r="S39" s="8"/>
@@ -1954,7 +1964,7 @@
       </c>
       <c r="P40" s="6"/>
       <c r="Q40" s="4">
-        <f>C40+D40+E40+F40+G40+H40+I40+J40+K40+L40+M40+N40+O40+P40</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="R40" s="7"/>
@@ -1974,7 +1984,7 @@
       <c r="J41" s="16"/>
       <c r="P41" s="6"/>
       <c r="Q41" s="4">
-        <f>C41+D41+E41+F41+G41+H41+I41+J41+K41+L41+M41+N41+O41+P41</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="R41" s="9"/>
@@ -1984,7 +1994,9 @@
       <c r="B42" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C42" s="5"/>
+      <c r="C42" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="D42" t="b">
         <v>1</v>
       </c>
@@ -2008,8 +2020,8 @@
       </c>
       <c r="P42" s="6"/>
       <c r="Q42" s="4">
-        <f>C42+D42+E42+F42+G42+H42+I42+J42+K42+L42+M42+N42+O42+P42</f>
-        <v>7</v>
+        <f t="shared" si="1"/>
+        <v>8</v>
       </c>
       <c r="R42" s="7"/>
       <c r="S42" s="8"/>
@@ -2028,7 +2040,7 @@
       <c r="J43" s="16"/>
       <c r="P43" s="6"/>
       <c r="Q43" s="4">
-        <f>C43+D43+E43+F43+G43+H43+I43+J43+K43+L43+M43+N43+O43+P43</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="R43" s="7"/>
@@ -2054,11 +2066,13 @@
       <c r="I44" t="b">
         <v>1</v>
       </c>
-      <c r="J44" s="16"/>
+      <c r="J44" s="16" t="b">
+        <v>1</v>
+      </c>
       <c r="P44" s="6"/>
       <c r="Q44" s="4">
-        <f>C44+D44+E44+F44+G44+H44+I44+J44+K44+L44+M44+N44+O44+P44</f>
-        <v>5</v>
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="R44" s="7"/>
       <c r="S44" s="8"/>
@@ -2090,7 +2104,7 @@
       </c>
       <c r="P45" s="6"/>
       <c r="Q45" s="4">
-        <f>C45+D45+E45+F45+G45+H45+I45+J45+K45+L45+M45+N45+O45+P45</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="R45" s="7"/>
@@ -2113,7 +2127,7 @@
       <c r="J46" s="16"/>
       <c r="P46" s="6"/>
       <c r="Q46" s="4">
-        <f>C46+D46+E46+F46+G46+H46+I46+J46+K46+L46+M46+N46+O46+P46</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="R46" s="7"/>
@@ -2138,7 +2152,7 @@
       </c>
       <c r="P47" s="6"/>
       <c r="Q47" s="4">
-        <f>C47+D47+E47+F47+G47+H47+I47+J47+K47+L47+M47+N47+O47+P47</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="R47" s="7"/>
@@ -2165,7 +2179,7 @@
       </c>
       <c r="P48" s="6"/>
       <c r="Q48" s="4">
-        <f>C48+D48+E48+F48+G48+H48+I48+J48+K48+L48+M48+N48+O48+P48</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="R48" s="9"/>
@@ -2196,7 +2210,7 @@
       </c>
       <c r="P49" s="6"/>
       <c r="Q49" s="4">
-        <f>C49+D49+E49+F49+G49+H49+I49+J49+K49+L49+M49+N49+O49+P49</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="R49" s="7"/>
@@ -2225,11 +2239,13 @@
       <c r="I50" t="b">
         <v>1</v>
       </c>
-      <c r="J50" s="16"/>
+      <c r="J50" s="16" t="b">
+        <v>1</v>
+      </c>
       <c r="P50" s="6"/>
       <c r="Q50" s="4">
-        <f>C50+D50+E50+F50+G50+H50+I50+J50+K50+L50+M50+N50+O50+P50</f>
-        <v>6</v>
+        <f t="shared" si="1"/>
+        <v>7</v>
       </c>
       <c r="R50" s="7"/>
       <c r="S50" s="8"/>
@@ -2254,11 +2270,13 @@
       <c r="H51" t="b">
         <v>1</v>
       </c>
-      <c r="J51" s="16"/>
+      <c r="J51" s="16" t="b">
+        <v>1</v>
+      </c>
       <c r="P51" s="6"/>
       <c r="Q51" s="4">
-        <f>C51+D51+E51+F51+G51+H51+I51+J51+K51+L51+M51+N51+O51+P51</f>
-        <v>5</v>
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="R51" s="7"/>
       <c r="S51" s="8"/>
@@ -2277,7 +2295,7 @@
       <c r="J52" s="16"/>
       <c r="P52" s="6"/>
       <c r="Q52" s="4">
-        <f>C52+D52+E52+F52+G52+H52+I52+J52+K52+L52+M52+N52+O52+P52</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="R52" s="7"/>
@@ -2297,11 +2315,13 @@
       <c r="I53" t="b">
         <v>1</v>
       </c>
-      <c r="J53" s="16"/>
+      <c r="J53" s="16" t="b">
+        <v>1</v>
+      </c>
       <c r="P53" s="6"/>
       <c r="Q53" s="4">
-        <f>C53+D53+E53+F53+G53+H53+I53+J53+K53+L53+M53+N53+O53+P53</f>
-        <v>3</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="R53" s="7"/>
       <c r="S53" s="8"/>
@@ -2331,7 +2351,7 @@
       </c>
       <c r="P54" s="6"/>
       <c r="Q54" s="4">
-        <f>C54+D54+E54+F54+G54+H54+I54+J54+K54+L54+M54+N54+O54+P54</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="R54" s="7"/>
@@ -2348,7 +2368,7 @@
       <c r="J55" s="16"/>
       <c r="P55" s="6"/>
       <c r="Q55" s="4">
-        <f>C55+D55+E55+F55+G55+H55+I55+J55+K55+L55+M55+N55+O55+P55</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="R55" s="7"/>
@@ -2373,7 +2393,7 @@
       </c>
       <c r="P56" s="6"/>
       <c r="Q56" s="4">
-        <f>C56+D56+E56+F56+G56+H56+I56+J56+K56+L56+M56+N56+O56+P56</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="R56" s="7"/>
@@ -2407,8 +2427,8 @@
       <c r="N57" s="16"/>
       <c r="O57" s="16"/>
       <c r="P57" s="16"/>
-      <c r="Q57" s="35">
-        <f>C57+D57+E57+F57+G57+H57+I57+J57+K57+L57+M57+N57+O57+P57</f>
+      <c r="Q57" s="34">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="R57" s="23"/>
@@ -2435,16 +2455,18 @@
         <v>1</v>
       </c>
       <c r="I58" s="11"/>
-      <c r="J58" s="20"/>
+      <c r="J58" s="20" t="b">
+        <v>1</v>
+      </c>
       <c r="K58" s="11"/>
       <c r="L58" s="11"/>
       <c r="M58" s="11"/>
       <c r="N58" s="11"/>
       <c r="O58" s="11"/>
       <c r="P58" s="11"/>
-      <c r="Q58" s="35">
-        <f>C58+D58+E58+F58+G58+H58+I58+J58+K58+L58+M58+N58+O58+P58</f>
-        <v>5</v>
+      <c r="Q58" s="34">
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="R58" s="12"/>
       <c r="S58" s="13"/>

</xml_diff>

<commit_message>
curbe bezier pentru desenarea graficului cu mai multe muchii intre aceleasi noduri
</commit_message>
<xml_diff>
--- a/MetodeAvansateDeProgramare/Prezenta_AnII_2024.xlsx
+++ b/MetodeAvansateDeProgramare/Prezenta_AnII_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_Promotia_2023_2026\MetodeAvansateDeProgramare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F98AB062-0D21-4D5A-8856-C85C7AF216C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C51EBD9-07FF-40CE-A470-107E80D58302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
   <si>
     <t>Proiect</t>
   </si>
@@ -247,6 +247,9 @@
   </si>
   <si>
     <t>David Nadis</t>
+  </si>
+  <si>
+    <t>Cristea Octavian</t>
   </si>
 </sst>
 </file>
@@ -502,7 +505,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -582,6 +585,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -873,13 +879,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:S58"/>
+  <dimension ref="B2:S59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C51" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L19" sqref="L19"/>
+      <selection pane="bottomRight" activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1077,10 +1083,13 @@
         <v>1</v>
       </c>
       <c r="J7" s="16"/>
+      <c r="K7" t="b">
+        <v>1</v>
+      </c>
       <c r="P7" s="6"/>
       <c r="Q7" s="4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R7" s="7"/>
       <c r="S7" s="8"/>
@@ -1098,10 +1107,13 @@
       <c r="J8" s="16" t="b">
         <v>1</v>
       </c>
+      <c r="K8" t="b">
+        <v>1</v>
+      </c>
       <c r="P8" s="6"/>
       <c r="Q8" s="4">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R8" s="7"/>
       <c r="S8" s="8"/>
@@ -1129,10 +1141,13 @@
       <c r="J9" s="16" t="b">
         <v>1</v>
       </c>
+      <c r="K9" t="b">
+        <v>1</v>
+      </c>
       <c r="P9" s="6"/>
       <c r="Q9" s="4">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R9" s="7"/>
       <c r="S9" s="8"/>
@@ -1194,10 +1209,13 @@
         <v>1</v>
       </c>
       <c r="J12" s="16"/>
+      <c r="K12" t="b">
+        <v>1</v>
+      </c>
       <c r="P12" s="6"/>
       <c r="Q12" s="4">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R12" s="7"/>
       <c r="S12" s="8"/>
@@ -1260,10 +1278,13 @@
       <c r="J14" s="16" t="b">
         <v>1</v>
       </c>
+      <c r="K14" t="b">
+        <v>1</v>
+      </c>
       <c r="P14" s="6"/>
       <c r="Q14" s="4">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R14" s="7"/>
       <c r="S14" s="8"/>
@@ -1288,10 +1309,13 @@
       <c r="J15" s="16" t="b">
         <v>1</v>
       </c>
+      <c r="K15" t="b">
+        <v>1</v>
+      </c>
       <c r="P15" s="6"/>
       <c r="Q15" s="4">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R15" s="7"/>
       <c r="S15" s="8"/>
@@ -1322,10 +1346,13 @@
       <c r="J16" s="16" t="b">
         <v>1</v>
       </c>
+      <c r="K16" t="b">
+        <v>1</v>
+      </c>
       <c r="P16" s="6"/>
       <c r="Q16" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R16" s="9"/>
       <c r="S16" s="10"/>
@@ -1350,10 +1377,13 @@
       <c r="J17" s="16" t="b">
         <v>1</v>
       </c>
+      <c r="K17" t="b">
+        <v>1</v>
+      </c>
       <c r="P17" s="6"/>
       <c r="Q17" s="4">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R17" s="7"/>
       <c r="S17" s="8"/>
@@ -1384,10 +1414,13 @@
       <c r="J18" s="16" t="b">
         <v>1</v>
       </c>
+      <c r="K18" t="b">
+        <v>1</v>
+      </c>
       <c r="P18" s="6"/>
       <c r="Q18" s="4">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R18" s="7"/>
       <c r="S18" s="8"/>
@@ -1578,10 +1611,13 @@
       <c r="J25" s="16" t="b">
         <v>1</v>
       </c>
+      <c r="K25" t="b">
+        <v>1</v>
+      </c>
       <c r="P25" s="6"/>
       <c r="Q25" s="4">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R25" s="7"/>
       <c r="S25" s="8"/>
@@ -1597,10 +1633,13 @@
       <c r="J26" s="16" t="b">
         <v>1</v>
       </c>
+      <c r="K26" t="b">
+        <v>1</v>
+      </c>
       <c r="P26" s="6"/>
       <c r="Q26" s="4">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R26" s="7"/>
       <c r="S26" s="8"/>
@@ -1673,10 +1712,13 @@
       <c r="J29" s="16" t="b">
         <v>1</v>
       </c>
+      <c r="K29" t="b">
+        <v>1</v>
+      </c>
       <c r="P29" s="6"/>
       <c r="Q29" s="4">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R29" s="7"/>
       <c r="S29" s="8"/>
@@ -1833,7 +1875,7 @@
       </c>
       <c r="P35" s="6"/>
       <c r="Q35" s="4">
-        <f t="shared" ref="Q35:Q66" si="1">C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
+        <f t="shared" ref="Q35:Q59" si="1">C35+D35+E35+F35+G35+H35+I35+J35+K35+L35+M35+N35+O35+P35</f>
         <v>6</v>
       </c>
       <c r="R35" s="7"/>
@@ -1884,10 +1926,13 @@
       <c r="J37" s="16" t="b">
         <v>1</v>
       </c>
+      <c r="K37" t="b">
+        <v>1</v>
+      </c>
       <c r="P37" s="6"/>
       <c r="Q37" s="4">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R37" s="7"/>
       <c r="S37" s="8"/>
@@ -1918,10 +1963,13 @@
       <c r="J38" s="16" t="b">
         <v>1</v>
       </c>
+      <c r="K38" t="b">
+        <v>1</v>
+      </c>
       <c r="P38" s="6"/>
       <c r="Q38" s="4">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R38" s="7"/>
       <c r="S38" s="8"/>
@@ -2018,10 +2066,13 @@
       <c r="J42" s="16" t="b">
         <v>1</v>
       </c>
+      <c r="K42" t="b">
+        <v>1</v>
+      </c>
       <c r="P42" s="6"/>
       <c r="Q42" s="4">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R42" s="7"/>
       <c r="S42" s="8"/>
@@ -2150,10 +2201,13 @@
       <c r="J47" s="16" t="b">
         <v>1</v>
       </c>
+      <c r="K47" t="b">
+        <v>1</v>
+      </c>
       <c r="P47" s="6"/>
       <c r="Q47" s="4">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R47" s="7"/>
       <c r="S47" s="8"/>
@@ -2208,10 +2262,13 @@
       <c r="J49" s="16" t="b">
         <v>1</v>
       </c>
+      <c r="K49" t="b">
+        <v>1</v>
+      </c>
       <c r="P49" s="6"/>
       <c r="Q49" s="4">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R49" s="7"/>
       <c r="S49" s="8"/>
@@ -2349,10 +2406,13 @@
       <c r="J54" s="16" t="b">
         <v>1</v>
       </c>
+      <c r="K54" t="b">
+        <v>1</v>
+      </c>
       <c r="P54" s="6"/>
       <c r="Q54" s="4">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R54" s="7"/>
       <c r="S54" s="8"/>
@@ -2471,11 +2531,23 @@
       <c r="R58" s="12"/>
       <c r="S58" s="13"/>
     </row>
+    <row r="59" spans="2:19">
+      <c r="B59" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="K59" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q59" s="34">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:S58">
     <sortCondition ref="B3:B58"/>
   </sortState>
-  <conditionalFormatting sqref="Q3:Q58">
+  <conditionalFormatting sqref="Q3:Q59">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
       <formula>10</formula>
     </cfRule>

</xml_diff>

<commit_message>
stilizari + image upload
</commit_message>
<xml_diff>
--- a/MetodeAvansateDeProgramare/Prezenta_AnII_2024.xlsx
+++ b/MetodeAvansateDeProgramare/Prezenta_AnII_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_Promotia_2023_2026\MetodeAvansateDeProgramare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C51EBD9-07FF-40CE-A470-107E80D58302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F5678B3-D6FC-488E-B332-8ACEF8DB9CE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -882,10 +882,10 @@
   <dimension ref="B2:S59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C51" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D61" sqref="D61"/>
+      <selection pane="bottomRight" activeCell="K52" sqref="K52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1063,10 +1063,13 @@
       <c r="J6" s="16" t="b">
         <v>1</v>
       </c>
+      <c r="K6" t="b">
+        <v>1</v>
+      </c>
       <c r="P6" s="6"/>
       <c r="Q6" s="4">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R6" s="7"/>
       <c r="S6" s="8"/>
@@ -1208,14 +1211,16 @@
       <c r="I12" t="b">
         <v>1</v>
       </c>
-      <c r="J12" s="16"/>
+      <c r="J12" s="16" t="b">
+        <v>1</v>
+      </c>
       <c r="K12" t="b">
         <v>1</v>
       </c>
       <c r="P12" s="6"/>
       <c r="Q12" s="4">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R12" s="7"/>
       <c r="S12" s="8"/>
@@ -1242,7 +1247,9 @@
       <c r="J13" s="16" t="b">
         <v>1</v>
       </c>
-      <c r="K13" s="16"/>
+      <c r="K13" s="16" t="b">
+        <v>1</v>
+      </c>
       <c r="L13" s="16"/>
       <c r="M13" s="16"/>
       <c r="N13" s="16"/>
@@ -1250,7 +1257,7 @@
       <c r="P13" s="19"/>
       <c r="Q13" s="4">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R13" s="21"/>
       <c r="S13" s="22"/>
@@ -1324,7 +1331,9 @@
       <c r="B16" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="5"/>
+      <c r="C16" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="D16" t="b">
         <v>1</v>
       </c>
@@ -1352,7 +1361,7 @@
       <c r="P16" s="6"/>
       <c r="Q16" s="4">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R16" s="9"/>
       <c r="S16" s="10"/>
@@ -1578,7 +1587,9 @@
       <c r="J24" s="16" t="b">
         <v>1</v>
       </c>
-      <c r="K24" s="16"/>
+      <c r="K24" s="16" t="b">
+        <v>1</v>
+      </c>
       <c r="L24" s="16"/>
       <c r="M24" s="16"/>
       <c r="N24" s="16"/>
@@ -1586,7 +1597,7 @@
       <c r="P24" s="19"/>
       <c r="Q24" s="4">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R24" s="21"/>
       <c r="S24" s="28"/>
@@ -1630,6 +1641,9 @@
       <c r="G26" t="b">
         <v>1</v>
       </c>
+      <c r="I26" t="b">
+        <v>1</v>
+      </c>
       <c r="J26" s="16" t="b">
         <v>1</v>
       </c>
@@ -1639,7 +1653,7 @@
       <c r="P26" s="6"/>
       <c r="Q26" s="4">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R26" s="7"/>
       <c r="S26" s="8"/>
@@ -1768,10 +1782,13 @@
       <c r="J31" s="16" t="b">
         <v>1</v>
       </c>
+      <c r="K31" t="b">
+        <v>1</v>
+      </c>
       <c r="P31" s="6"/>
       <c r="Q31" s="4">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R31" s="9"/>
       <c r="S31" s="10"/>
@@ -1794,10 +1811,13 @@
         <v>1</v>
       </c>
       <c r="J32" s="16"/>
+      <c r="K32" t="b">
+        <v>1</v>
+      </c>
       <c r="P32" s="6"/>
       <c r="Q32" s="4">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R32" s="7"/>
       <c r="S32" s="8"/>
@@ -1842,10 +1862,13 @@
       <c r="J34" s="16" t="b">
         <v>1</v>
       </c>
+      <c r="K34" t="b">
+        <v>1</v>
+      </c>
       <c r="P34" s="6"/>
       <c r="Q34" s="4">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R34" s="7"/>
       <c r="S34" s="8"/>
@@ -1904,10 +1927,13 @@
       <c r="J36" s="16" t="b">
         <v>1</v>
       </c>
+      <c r="K36" t="b">
+        <v>1</v>
+      </c>
       <c r="P36" s="6"/>
       <c r="Q36" s="4">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R36" s="7"/>
       <c r="S36" s="8"/>
@@ -1991,10 +2017,13 @@
       <c r="J39" s="16" t="b">
         <v>1</v>
       </c>
+      <c r="K39" t="b">
+        <v>1</v>
+      </c>
       <c r="P39" s="6"/>
       <c r="Q39" s="4">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R39" s="7"/>
       <c r="S39" s="8"/>
@@ -2069,10 +2098,13 @@
       <c r="K42" t="b">
         <v>1</v>
       </c>
+      <c r="L42" t="b">
+        <v>1</v>
+      </c>
       <c r="P42" s="6"/>
       <c r="Q42" s="4">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="R42" s="7"/>
       <c r="S42" s="8"/>
@@ -2120,10 +2152,13 @@
       <c r="J44" s="16" t="b">
         <v>1</v>
       </c>
+      <c r="K44" t="b">
+        <v>1</v>
+      </c>
       <c r="P44" s="6"/>
       <c r="Q44" s="4">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R44" s="7"/>
       <c r="S44" s="8"/>
@@ -2189,6 +2224,9 @@
         <v>66</v>
       </c>
       <c r="C47" s="5"/>
+      <c r="F47" t="b">
+        <v>1</v>
+      </c>
       <c r="G47" t="b">
         <v>1</v>
       </c>
@@ -2207,7 +2245,7 @@
       <c r="P47" s="6"/>
       <c r="Q47" s="4">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R47" s="7"/>
       <c r="S47" s="8"/>
@@ -2231,10 +2269,13 @@
       <c r="J48" s="16" t="b">
         <v>1</v>
       </c>
+      <c r="K48" t="b">
+        <v>1</v>
+      </c>
       <c r="P48" s="6"/>
       <c r="Q48" s="4">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R48" s="9"/>
       <c r="S48" s="10"/>
@@ -2299,10 +2340,13 @@
       <c r="J50" s="16" t="b">
         <v>1</v>
       </c>
+      <c r="K50" t="b">
+        <v>1</v>
+      </c>
       <c r="P50" s="6"/>
       <c r="Q50" s="4">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R50" s="7"/>
       <c r="S50" s="8"/>
@@ -2330,10 +2374,13 @@
       <c r="J51" s="16" t="b">
         <v>1</v>
       </c>
+      <c r="K51" t="b">
+        <v>1</v>
+      </c>
       <c r="P51" s="6"/>
       <c r="Q51" s="4">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R51" s="7"/>
       <c r="S51" s="8"/>
@@ -2375,10 +2422,13 @@
       <c r="J53" s="16" t="b">
         <v>1</v>
       </c>
+      <c r="K53" t="b">
+        <v>1</v>
+      </c>
       <c r="P53" s="6"/>
       <c r="Q53" s="4">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R53" s="7"/>
       <c r="S53" s="8"/>
@@ -2518,7 +2568,9 @@
       <c r="J58" s="20" t="b">
         <v>1</v>
       </c>
-      <c r="K58" s="11"/>
+      <c r="K58" s="11" t="b">
+        <v>1</v>
+      </c>
       <c r="L58" s="11"/>
       <c r="M58" s="11"/>
       <c r="N58" s="11"/>
@@ -2526,7 +2578,7 @@
       <c r="P58" s="11"/>
       <c r="Q58" s="34">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R58" s="12"/>
       <c r="S58" s="13"/>

</xml_diff>